<commit_message>
Updated simulation files with Holden scheme
</commit_message>
<xml_diff>
--- a/JupyterNotebooks/AvgHW/Alpha1F-HW03.xlsx
+++ b/JupyterNotebooks/AvgHW/Alpha1F-HW03.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>HKL</t>
   </si>
@@ -58,6 +58,18 @@
     <t>OffsetATD</t>
   </si>
   <si>
+    <t>Holden2.5</t>
+  </si>
+  <si>
+    <t>Holden5</t>
+  </si>
+  <si>
+    <t>Holden10</t>
+  </si>
+  <si>
+    <t>Holden15</t>
+  </si>
+  <si>
     <t>HexGrid-90degTilt2.5degRes</t>
   </si>
   <si>
@@ -70,28 +82,28 @@
     <t>HexGrid-90degTilt15degRes</t>
   </si>
   <si>
+    <t>[2, 0, 0]</t>
+  </si>
+  <si>
+    <t>[2, 2, 0]</t>
+  </si>
+  <si>
+    <t>[2, 1, 1]</t>
+  </si>
+  <si>
+    <t>[4, 0, 0]</t>
+  </si>
+  <si>
+    <t>[3, 2, 1]</t>
+  </si>
+  <si>
     <t>[1, 1, 0]</t>
   </si>
   <si>
-    <t>[2, 0, 0]</t>
-  </si>
-  <si>
-    <t>[2, 1, 1]</t>
-  </si>
-  <si>
-    <t>[2, 2, 0]</t>
+    <t>[3, 1, 0]</t>
   </si>
   <si>
     <t>[2, 2, 2]</t>
-  </si>
-  <si>
-    <t>[3, 1, 0]</t>
-  </si>
-  <si>
-    <t>[3, 2, 1]</t>
-  </si>
-  <si>
-    <t>[4, 0, 0]</t>
   </si>
   <si>
     <t>1Pair-A</t>
@@ -479,7 +491,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T19"/>
+  <dimension ref="A1:T23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -552,58 +564,58 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="E2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="F2" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="G2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="H2" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="I2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="J2" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="K2" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="L2" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="M2" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="N2" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="O2" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="P2" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="Q2" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="R2" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="S2" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="T2" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:20">
@@ -614,28 +626,28 @@
         <v>1</v>
       </c>
       <c r="C3">
+        <v>0.9536650201154074</v>
+      </c>
+      <c r="D3">
         <v>1.152945834855813</v>
-      </c>
-      <c r="D3">
-        <v>0.9536650201154075</v>
       </c>
       <c r="E3">
         <v>0.937182945962484</v>
       </c>
       <c r="F3">
+        <v>0.9536650201154074</v>
+      </c>
+      <c r="G3">
+        <v>1.041997125837943</v>
+      </c>
+      <c r="H3">
         <v>1.152945834855813</v>
       </c>
-      <c r="G3">
+      <c r="I3">
+        <v>0.9422994293293789</v>
+      </c>
+      <c r="J3">
         <v>0.9432975636099349</v>
-      </c>
-      <c r="H3">
-        <v>0.9422994293293789</v>
-      </c>
-      <c r="I3">
-        <v>1.041997125837943</v>
-      </c>
-      <c r="J3">
-        <v>0.9536650201154075</v>
       </c>
       <c r="K3">
         <v>1.152945834855813</v>
@@ -665,7 +677,7 @@
         <v>1.049184908947379</v>
       </c>
       <c r="T3">
-        <v>0.9952313199518269</v>
+        <v>0.9952313199518268</v>
       </c>
     </row>
     <row r="4" spans="1:20">
@@ -676,28 +688,28 @@
         <v>2</v>
       </c>
       <c r="C4">
+        <v>1.225419474706893</v>
+      </c>
+      <c r="D4">
         <v>1.291315184167343</v>
-      </c>
-      <c r="D4">
-        <v>1.225419474706893</v>
       </c>
       <c r="E4">
         <v>0.9281919766583274</v>
       </c>
       <c r="F4">
+        <v>1.225419474706893</v>
+      </c>
+      <c r="G4">
+        <v>1.143606536477421</v>
+      </c>
+      <c r="H4">
         <v>1.291315184167343</v>
       </c>
-      <c r="G4">
+      <c r="I4">
+        <v>0.7039957044935053</v>
+      </c>
+      <c r="J4">
         <v>1.008385953488546</v>
-      </c>
-      <c r="H4">
-        <v>0.7039957044935053</v>
-      </c>
-      <c r="I4">
-        <v>1.143606536477421</v>
-      </c>
-      <c r="J4">
-        <v>1.225419474706893</v>
       </c>
       <c r="K4">
         <v>1.291315184167343</v>
@@ -738,28 +750,28 @@
         <v>3</v>
       </c>
       <c r="C5">
+        <v>0.1288273206544606</v>
+      </c>
+      <c r="D5">
         <v>2.051584262501862</v>
-      </c>
-      <c r="D5">
-        <v>0.1288273206544606</v>
       </c>
       <c r="E5">
         <v>0.9885706214910599</v>
       </c>
       <c r="F5">
+        <v>0.1288273206544606</v>
+      </c>
+      <c r="G5">
+        <v>1.664477351232213</v>
+      </c>
+      <c r="H5">
         <v>2.051584262501862</v>
       </c>
-      <c r="G5">
-        <v>0.6813256377537013</v>
-      </c>
-      <c r="H5">
-        <v>0.6793054559236139</v>
-      </c>
       <c r="I5">
-        <v>1.664477351232213</v>
+        <v>0.679305455923614</v>
       </c>
       <c r="J5">
-        <v>0.1288273206544606</v>
+        <v>0.6813256377537009</v>
       </c>
       <c r="K5">
         <v>2.051584262501862</v>
@@ -800,28 +812,28 @@
         <v>4</v>
       </c>
       <c r="C6">
+        <v>-0.0001886089917827399</v>
+      </c>
+      <c r="D6">
         <v>4.218585539063117</v>
-      </c>
-      <c r="D6">
-        <v>-0.00018860899178274</v>
       </c>
       <c r="E6">
         <v>0.03829107386291899</v>
       </c>
       <c r="F6">
+        <v>-0.0001886089917827399</v>
+      </c>
+      <c r="G6">
+        <v>1.343956095415291</v>
+      </c>
+      <c r="H6">
         <v>4.218585539063117</v>
       </c>
-      <c r="G6">
+      <c r="I6">
+        <v>0.5955406690348662</v>
+      </c>
+      <c r="J6">
         <v>1.903788088321897</v>
-      </c>
-      <c r="H6">
-        <v>0.5955406690348662</v>
-      </c>
-      <c r="I6">
-        <v>1.343956095415291</v>
-      </c>
-      <c r="J6">
-        <v>-0.00018860899178274</v>
       </c>
       <c r="K6">
         <v>4.218585539063117</v>
@@ -862,31 +874,31 @@
         <v>5</v>
       </c>
       <c r="C7">
-        <v>1.047986879235474</v>
+        <v>1.019959256811309</v>
       </c>
       <c r="D7">
-        <v>1.01995925681131</v>
+        <v>1.047986879235471</v>
       </c>
       <c r="E7">
         <v>0.9918784523322198</v>
       </c>
       <c r="F7">
-        <v>1.047986879235474</v>
+        <v>1.019959256811309</v>
       </c>
       <c r="G7">
+        <v>0.9925111675685032</v>
+      </c>
+      <c r="H7">
+        <v>1.047986879235471</v>
+      </c>
+      <c r="I7">
+        <v>0.9739851518986552</v>
+      </c>
+      <c r="J7">
         <v>1.024127889905488</v>
       </c>
-      <c r="H7">
-        <v>0.9739851518986554</v>
-      </c>
-      <c r="I7">
-        <v>0.9925111675685035</v>
-      </c>
-      <c r="J7">
-        <v>1.01995925681131</v>
-      </c>
       <c r="K7">
-        <v>1.047986879235474</v>
+        <v>1.047986879235471</v>
       </c>
       <c r="L7">
         <v>0.9918784523322198</v>
@@ -898,22 +910,22 @@
         <v>1.005918854571765</v>
       </c>
       <c r="O7">
-        <v>0.9952742870140616</v>
+        <v>0.9952742870140615</v>
       </c>
       <c r="P7">
-        <v>1.019941529459668</v>
+        <v>1.019941529459667</v>
       </c>
       <c r="Q7">
-        <v>1.019941529459668</v>
+        <v>1.019941529459667</v>
       </c>
       <c r="R7">
-        <v>1.026952866903619</v>
+        <v>1.026952866903618</v>
       </c>
       <c r="S7">
-        <v>1.026952866903619</v>
+        <v>1.026952866903618</v>
       </c>
       <c r="T7">
-        <v>1.008408132958609</v>
+        <v>1.008408132958608</v>
       </c>
     </row>
     <row r="8" spans="1:20">
@@ -924,58 +936,58 @@
         <v>6</v>
       </c>
       <c r="C8">
-        <v>1.091641707993743</v>
+        <v>1.034234591157339</v>
       </c>
       <c r="D8">
-        <v>1.034234591157332</v>
+        <v>1.091641707993742</v>
       </c>
       <c r="E8">
-        <v>0.98690271337804</v>
+        <v>0.9869027133780399</v>
       </c>
       <c r="F8">
-        <v>1.091641707993743</v>
+        <v>1.034234591157339</v>
       </c>
       <c r="G8">
-        <v>1.022593623954923</v>
+        <v>0.9874922857148483</v>
       </c>
       <c r="H8">
+        <v>1.091641707993742</v>
+      </c>
+      <c r="I8">
         <v>0.9740675218658092</v>
       </c>
-      <c r="I8">
-        <v>0.9874922857148486</v>
-      </c>
       <c r="J8">
-        <v>1.034234591157332</v>
+        <v>1.022593623954924</v>
       </c>
       <c r="K8">
-        <v>1.091641707993743</v>
+        <v>1.091641707993742</v>
       </c>
       <c r="L8">
-        <v>0.98690271337804</v>
+        <v>0.9869027133780399</v>
       </c>
       <c r="M8">
-        <v>1.010568652267686</v>
+        <v>1.010568652267689</v>
       </c>
       <c r="N8">
-        <v>1.010568652267686</v>
+        <v>1.010568652267689</v>
       </c>
       <c r="O8">
-        <v>0.9984016088003939</v>
+        <v>0.9984016088003959</v>
       </c>
       <c r="P8">
-        <v>1.037593004176372</v>
+        <v>1.037593004176374</v>
       </c>
       <c r="Q8">
-        <v>1.037593004176372</v>
+        <v>1.037593004176374</v>
       </c>
       <c r="R8">
-        <v>1.051105180130715</v>
+        <v>1.051105180130716</v>
       </c>
       <c r="S8">
-        <v>1.051105180130715</v>
+        <v>1.051105180130716</v>
       </c>
       <c r="T8">
-        <v>1.016155407344116</v>
+        <v>1.016155407344117</v>
       </c>
     </row>
     <row r="9" spans="1:20">
@@ -986,34 +998,34 @@
         <v>7</v>
       </c>
       <c r="C9">
+        <v>0.967546277645851</v>
+      </c>
+      <c r="D9">
         <v>1.258806238220695</v>
       </c>
-      <c r="D9">
-        <v>0.9675462776458512</v>
-      </c>
       <c r="E9">
-        <v>0.9693562270106392</v>
+        <v>0.9693562270106393</v>
       </c>
       <c r="F9">
+        <v>0.967546277645851</v>
+      </c>
+      <c r="G9">
+        <v>0.9729641384379286</v>
+      </c>
+      <c r="H9">
         <v>1.258806238220695</v>
       </c>
-      <c r="G9">
+      <c r="I9">
+        <v>0.9603048457350022</v>
+      </c>
+      <c r="J9">
         <v>0.9783919335572949</v>
-      </c>
-      <c r="H9">
-        <v>0.9603048457350024</v>
-      </c>
-      <c r="I9">
-        <v>0.9729641384379286</v>
-      </c>
-      <c r="J9">
-        <v>0.9675462776458512</v>
       </c>
       <c r="K9">
         <v>1.258806238220695</v>
       </c>
       <c r="L9">
-        <v>0.9693562270106392</v>
+        <v>0.9693562270106393</v>
       </c>
       <c r="M9">
         <v>0.9684512523282451</v>
@@ -1048,28 +1060,28 @@
         <v>8</v>
       </c>
       <c r="C10">
+        <v>1.018142314512956</v>
+      </c>
+      <c r="D10">
         <v>1.534687420495374</v>
-      </c>
-      <c r="D10">
-        <v>1.018142314512956</v>
       </c>
       <c r="E10">
         <v>1.062993573522152</v>
       </c>
       <c r="F10">
+        <v>1.018142314512956</v>
+      </c>
+      <c r="G10">
+        <v>1.063100811713334</v>
+      </c>
+      <c r="H10">
         <v>1.534687420495374</v>
       </c>
-      <c r="G10">
+      <c r="I10">
+        <v>0.8590858623377114</v>
+      </c>
+      <c r="J10">
         <v>1.110109093028632</v>
-      </c>
-      <c r="H10">
-        <v>0.8590858623377114</v>
-      </c>
-      <c r="I10">
-        <v>1.063100811713334</v>
-      </c>
-      <c r="J10">
-        <v>1.018142314512956</v>
       </c>
       <c r="K10">
         <v>1.534687420495374</v>
@@ -1084,7 +1096,7 @@
         <v>1.040567944017554</v>
       </c>
       <c r="O10">
-        <v>0.9800739167909399</v>
+        <v>0.9800739167909397</v>
       </c>
       <c r="P10">
         <v>1.205274436176827</v>
@@ -1099,7 +1111,7 @@
         <v>1.287627682256464</v>
       </c>
       <c r="T10">
-        <v>1.108019845935027</v>
+        <v>1.108019845935026</v>
       </c>
     </row>
     <row r="11" spans="1:20">
@@ -1110,34 +1122,34 @@
         <v>9</v>
       </c>
       <c r="C11">
+        <v>1.199301118019966</v>
+      </c>
+      <c r="D11">
         <v>2.333464727294784</v>
       </c>
-      <c r="D11">
+      <c r="E11">
+        <v>0.8213258604366269</v>
+      </c>
+      <c r="F11">
         <v>1.199301118019966</v>
       </c>
-      <c r="E11">
-        <v>0.8213258604366268</v>
-      </c>
-      <c r="F11">
+      <c r="G11">
+        <v>0.9523004446201929</v>
+      </c>
+      <c r="H11">
         <v>2.333464727294784</v>
       </c>
-      <c r="G11">
+      <c r="I11">
+        <v>0.8342399679404154</v>
+      </c>
+      <c r="J11">
         <v>0.6087295150139962</v>
-      </c>
-      <c r="H11">
-        <v>0.8342399679404157</v>
-      </c>
-      <c r="I11">
-        <v>0.9523004446201929</v>
-      </c>
-      <c r="J11">
-        <v>1.199301118019966</v>
       </c>
       <c r="K11">
         <v>2.333464727294784</v>
       </c>
       <c r="L11">
-        <v>0.8213258604366268</v>
+        <v>0.8213258604366269</v>
       </c>
       <c r="M11">
         <v>1.010313489228296</v>
@@ -1172,49 +1184,49 @@
         <v>10</v>
       </c>
       <c r="C12">
+        <v>0.0009906382284935978</v>
+      </c>
+      <c r="D12">
         <v>1.650333686930785</v>
       </c>
-      <c r="D12">
-        <v>0.0009906382284935974</v>
-      </c>
       <c r="E12">
-        <v>0.9268749225926884</v>
+        <v>0.9268749225926886</v>
       </c>
       <c r="F12">
+        <v>0.0009906382284935978</v>
+      </c>
+      <c r="G12">
+        <v>2.22350904549545</v>
+      </c>
+      <c r="H12">
         <v>1.650333686930785</v>
       </c>
-      <c r="G12">
-        <v>0.001147664018377606</v>
-      </c>
-      <c r="H12">
-        <v>1.891613563536644</v>
-      </c>
       <c r="I12">
-        <v>2.223509045495451</v>
+        <v>1.891613563536645</v>
       </c>
       <c r="J12">
-        <v>0.0009906382284935974</v>
+        <v>0.001147664018377604</v>
       </c>
       <c r="K12">
         <v>1.650333686930785</v>
       </c>
       <c r="L12">
-        <v>0.9268749225926884</v>
+        <v>0.9268749225926886</v>
       </c>
       <c r="M12">
-        <v>0.463932780410591</v>
+        <v>0.4639327804105911</v>
       </c>
       <c r="N12">
-        <v>0.463932780410591</v>
+        <v>0.4639327804105911</v>
       </c>
       <c r="O12">
         <v>0.9398263747859422</v>
       </c>
       <c r="P12">
-        <v>0.8593997492506555</v>
+        <v>0.8593997492506559</v>
       </c>
       <c r="Q12">
-        <v>0.8593997492506557</v>
+        <v>0.8593997492506559</v>
       </c>
       <c r="R12">
         <v>1.057133233670688</v>
@@ -1234,58 +1246,58 @@
         <v>11</v>
       </c>
       <c r="C13">
-        <v>0.7953816718760839</v>
+        <v>3.806806310651667</v>
       </c>
       <c r="D13">
-        <v>3.806806310651665</v>
+        <v>0.795381671876087</v>
       </c>
       <c r="E13">
-        <v>1.257223936975513</v>
+        <v>1.257223936975514</v>
       </c>
       <c r="F13">
-        <v>0.7953816718760839</v>
+        <v>3.806806310651667</v>
       </c>
       <c r="G13">
-        <v>2.492586044649236</v>
+        <v>1.380876313850261</v>
       </c>
       <c r="H13">
-        <v>1.878161985072148</v>
+        <v>0.795381671876087</v>
       </c>
       <c r="I13">
-        <v>1.380876313850262</v>
+        <v>1.878161985072147</v>
       </c>
       <c r="J13">
-        <v>3.806806310651665</v>
+        <v>2.492586044649239</v>
       </c>
       <c r="K13">
-        <v>0.7953816718760839</v>
+        <v>0.795381671876087</v>
       </c>
       <c r="L13">
-        <v>1.257223936975513</v>
+        <v>1.257223936975514</v>
       </c>
       <c r="M13">
-        <v>2.532015123813589</v>
+        <v>2.532015123813591</v>
       </c>
       <c r="N13">
-        <v>2.532015123813589</v>
+        <v>2.532015123813591</v>
       </c>
       <c r="O13">
-        <v>2.314064077566442</v>
+        <v>2.314064077566443</v>
       </c>
       <c r="P13">
-        <v>1.953137306501087</v>
+        <v>1.95313730650109</v>
       </c>
       <c r="Q13">
-        <v>1.953137306501087</v>
+        <v>1.953137306501089</v>
       </c>
       <c r="R13">
-        <v>1.663698397844836</v>
+        <v>1.663698397844839</v>
       </c>
       <c r="S13">
-        <v>1.663698397844836</v>
+        <v>1.663698397844839</v>
       </c>
       <c r="T13">
-        <v>1.935172710512485</v>
+        <v>1.935172710512486</v>
       </c>
     </row>
     <row r="14" spans="1:20">
@@ -1296,58 +1308,58 @@
         <v>12</v>
       </c>
       <c r="C14">
-        <v>-0.0007584295794183397</v>
+        <v>0.5490285290253076</v>
       </c>
       <c r="D14">
-        <v>0.549028529025309</v>
+        <v>-0.000758429579418342</v>
       </c>
       <c r="E14">
-        <v>1.694874496173249</v>
+        <v>1.694874496173247</v>
       </c>
       <c r="F14">
-        <v>-0.0007584295794183397</v>
+        <v>0.5490285290253076</v>
       </c>
       <c r="G14">
-        <v>0.07992494560801593</v>
+        <v>0.09679846039972893</v>
       </c>
       <c r="H14">
+        <v>-0.000758429579418342</v>
+      </c>
+      <c r="I14">
         <v>2.163906465814728</v>
       </c>
-      <c r="I14">
-        <v>0.09679846039972904</v>
-      </c>
       <c r="J14">
-        <v>0.549028529025309</v>
+        <v>0.07992494560801601</v>
       </c>
       <c r="K14">
-        <v>-0.0007584295794183397</v>
+        <v>-0.000758429579418342</v>
       </c>
       <c r="L14">
-        <v>1.694874496173249</v>
+        <v>1.694874496173247</v>
       </c>
       <c r="M14">
-        <v>1.121951512599279</v>
+        <v>1.121951512599277</v>
       </c>
       <c r="N14">
-        <v>1.121951512599279</v>
+        <v>1.121951512599277</v>
       </c>
       <c r="O14">
-        <v>1.469269830337762</v>
+        <v>1.469269830337761</v>
       </c>
       <c r="P14">
-        <v>0.74771486520638</v>
+        <v>0.7477148652063786</v>
       </c>
       <c r="Q14">
-        <v>0.74771486520638</v>
+        <v>0.7477148652063788</v>
       </c>
       <c r="R14">
-        <v>0.5605965415099303</v>
+        <v>0.5605965415099294</v>
       </c>
       <c r="S14">
-        <v>0.5605965415099303</v>
+        <v>0.5605965415099294</v>
       </c>
       <c r="T14">
-        <v>0.7639624112402689</v>
+        <v>0.763962411240268</v>
       </c>
     </row>
     <row r="15" spans="1:20">
@@ -1358,31 +1370,31 @@
         <v>13</v>
       </c>
       <c r="C15">
-        <v>0.07529789264772961</v>
+        <v>0.06949281876991974</v>
       </c>
       <c r="D15">
-        <v>0.06949281876991974</v>
+        <v>0.07529789264772963</v>
       </c>
       <c r="E15">
         <v>0.4828810263023473</v>
       </c>
       <c r="F15">
-        <v>0.07529789264772961</v>
+        <v>0.06949281876991974</v>
       </c>
       <c r="G15">
+        <v>1.401767971530121</v>
+      </c>
+      <c r="H15">
+        <v>0.07529789264772963</v>
+      </c>
+      <c r="I15">
+        <v>-0.0004574272900550851</v>
+      </c>
+      <c r="J15">
         <v>0.01587949993991768</v>
       </c>
-      <c r="H15">
-        <v>-0.0004574272900550843</v>
-      </c>
-      <c r="I15">
-        <v>1.401767971530122</v>
-      </c>
-      <c r="J15">
-        <v>0.06949281876991974</v>
-      </c>
       <c r="K15">
-        <v>0.07529789264772961</v>
+        <v>0.07529789264772963</v>
       </c>
       <c r="L15">
         <v>0.4828810263023473</v>
@@ -1397,16 +1409,16 @@
         <v>0.1839721392607373</v>
       </c>
       <c r="P15">
-        <v>0.2092239125733322</v>
+        <v>0.2092239125733323</v>
       </c>
       <c r="Q15">
-        <v>0.2092239125733322</v>
+        <v>0.2092239125733323</v>
       </c>
       <c r="R15">
-        <v>0.1757424075919315</v>
+        <v>0.1757424075919316</v>
       </c>
       <c r="S15">
-        <v>0.1757424075919315</v>
+        <v>0.1757424075919316</v>
       </c>
       <c r="T15">
         <v>0.3408102969833302</v>
@@ -1420,58 +1432,58 @@
         <v>14</v>
       </c>
       <c r="C16">
-        <v>1.007149811752503</v>
+        <v>0.3085601364342757</v>
       </c>
       <c r="D16">
-        <v>1.027173618904952</v>
+        <v>3.071795639929197</v>
       </c>
       <c r="E16">
-        <v>0.9934485654429699</v>
+        <v>0.217506328328065</v>
       </c>
       <c r="F16">
-        <v>1.007149811752503</v>
+        <v>0.3085601364342757</v>
       </c>
       <c r="G16">
-        <v>1.029531886213101</v>
+        <v>1.592594248146821</v>
       </c>
       <c r="H16">
-        <v>0.9740750792802707</v>
+        <v>3.071795639929197</v>
       </c>
       <c r="I16">
-        <v>0.9949796103605598</v>
+        <v>0.2902399871761469</v>
       </c>
       <c r="J16">
-        <v>1.027173618904952</v>
+        <v>0.2053299211491966</v>
       </c>
       <c r="K16">
-        <v>1.007149811752503</v>
+        <v>3.071795639929197</v>
       </c>
       <c r="L16">
-        <v>0.9934485654429699</v>
+        <v>0.217506328328065</v>
       </c>
       <c r="M16">
-        <v>1.010311092173961</v>
+        <v>0.2630332323811704</v>
       </c>
       <c r="N16">
-        <v>1.010311092173961</v>
+        <v>0.2630332323811704</v>
       </c>
       <c r="O16">
-        <v>0.9982324212093977</v>
+        <v>0.2721021506461626</v>
       </c>
       <c r="P16">
-        <v>1.009257332033475</v>
+        <v>1.199287368230513</v>
       </c>
       <c r="Q16">
-        <v>1.009257332033475</v>
+        <v>1.199287368230513</v>
       </c>
       <c r="R16">
-        <v>1.008730451963232</v>
+        <v>1.667414436155184</v>
       </c>
       <c r="S16">
-        <v>1.008730451963232</v>
+        <v>1.667414436155184</v>
       </c>
       <c r="T16">
-        <v>1.004393095325726</v>
+        <v>0.9476710435272837</v>
       </c>
     </row>
     <row r="17" spans="1:20">
@@ -1482,58 +1494,58 @@
         <v>15</v>
       </c>
       <c r="C17">
-        <v>1.142308003872337</v>
+        <v>0.6217695547943317</v>
       </c>
       <c r="D17">
-        <v>0.972213077140635</v>
+        <v>2.37731836298703</v>
       </c>
       <c r="E17">
-        <v>0.9856795263322907</v>
+        <v>0.433627980337418</v>
       </c>
       <c r="F17">
-        <v>1.142308003872337</v>
+        <v>0.6217695547943317</v>
       </c>
       <c r="G17">
-        <v>1.02187662150615</v>
+        <v>1.34738564824695</v>
       </c>
       <c r="H17">
-        <v>0.9623569163749013</v>
+        <v>2.37731836298703</v>
       </c>
       <c r="I17">
-        <v>1.007890703643512</v>
+        <v>0.5536156664368842</v>
       </c>
       <c r="J17">
-        <v>0.972213077140635</v>
+        <v>0.4100638425572888</v>
       </c>
       <c r="K17">
-        <v>1.142308003872337</v>
+        <v>2.37731836298703</v>
       </c>
       <c r="L17">
-        <v>0.9856795263322907</v>
+        <v>0.433627980337418</v>
       </c>
       <c r="M17">
-        <v>0.9789463017364628</v>
+        <v>0.5276987675658749</v>
       </c>
       <c r="N17">
-        <v>0.9789463017364628</v>
+        <v>0.5276987675658749</v>
       </c>
       <c r="O17">
-        <v>0.9734165066159424</v>
+        <v>0.5363377338562113</v>
       </c>
       <c r="P17">
-        <v>1.033400202448421</v>
+        <v>1.14423863270626</v>
       </c>
       <c r="Q17">
-        <v>1.033400202448421</v>
+        <v>1.14423863270626</v>
       </c>
       <c r="R17">
-        <v>1.0606271528044</v>
+        <v>1.452508565276452</v>
       </c>
       <c r="S17">
-        <v>1.0606271528044</v>
+        <v>1.452508565276452</v>
       </c>
       <c r="T17">
-        <v>1.015387474811638</v>
+        <v>0.9572968425599836</v>
       </c>
     </row>
     <row r="18" spans="1:20">
@@ -1544,58 +1556,58 @@
         <v>16</v>
       </c>
       <c r="C18">
-        <v>2.392977173124852</v>
+        <v>0.9820973821532326</v>
       </c>
       <c r="D18">
-        <v>1.457039515344586</v>
+        <v>1.235184147443256</v>
       </c>
       <c r="E18">
-        <v>0.9010736078904343</v>
+        <v>0.9143758656787601</v>
       </c>
       <c r="F18">
-        <v>2.392977173124852</v>
+        <v>0.9820973821532326</v>
       </c>
       <c r="G18">
-        <v>0.9287588546661991</v>
+        <v>0.6963413652154223</v>
       </c>
       <c r="H18">
-        <v>0.9293525787020404</v>
+        <v>1.235184147443256</v>
       </c>
       <c r="I18">
-        <v>1.23795400321317</v>
+        <v>1.063769582472242</v>
       </c>
       <c r="J18">
-        <v>1.457039515344586</v>
+        <v>1.178966652121838</v>
       </c>
       <c r="K18">
-        <v>2.392977173124852</v>
+        <v>1.235184147443256</v>
       </c>
       <c r="L18">
-        <v>0.9010736078904343</v>
+        <v>0.9143758656787601</v>
       </c>
       <c r="M18">
-        <v>1.17905656161751</v>
+        <v>0.9482366239159963</v>
       </c>
       <c r="N18">
-        <v>1.17905656161751</v>
+        <v>0.9482366239159963</v>
       </c>
       <c r="O18">
-        <v>1.095821900645687</v>
+        <v>0.9867476101014114</v>
       </c>
       <c r="P18">
-        <v>1.583696765453291</v>
+        <v>1.043885798425083</v>
       </c>
       <c r="Q18">
-        <v>1.583696765453291</v>
+        <v>1.043885798425083</v>
       </c>
       <c r="R18">
-        <v>1.786016867371181</v>
+        <v>1.091710385679626</v>
       </c>
       <c r="S18">
-        <v>1.786016867371181</v>
+        <v>1.091710385679626</v>
       </c>
       <c r="T18">
-        <v>1.307859288823547</v>
+        <v>1.011789165847458</v>
       </c>
     </row>
     <row r="19" spans="1:20">
@@ -1606,57 +1618,305 @@
         <v>17</v>
       </c>
       <c r="C19">
+        <v>1.218431711863248</v>
+      </c>
+      <c r="D19">
+        <v>0.9629614397539579</v>
+      </c>
+      <c r="E19">
+        <v>0.653680419195017</v>
+      </c>
+      <c r="F19">
+        <v>1.218431711863248</v>
+      </c>
+      <c r="G19">
+        <v>1.045995082310377</v>
+      </c>
+      <c r="H19">
+        <v>0.9629614397539579</v>
+      </c>
+      <c r="I19">
+        <v>0.9353360884254763</v>
+      </c>
+      <c r="J19">
+        <v>1.011351423487716</v>
+      </c>
+      <c r="K19">
+        <v>0.9629614397539579</v>
+      </c>
+      <c r="L19">
+        <v>0.653680419195017</v>
+      </c>
+      <c r="M19">
+        <v>0.9360560655291323</v>
+      </c>
+      <c r="N19">
+        <v>0.9360560655291323</v>
+      </c>
+      <c r="O19">
+        <v>0.9358160731612469</v>
+      </c>
+      <c r="P19">
+        <v>0.9450245236040743</v>
+      </c>
+      <c r="Q19">
+        <v>0.9450245236040743</v>
+      </c>
+      <c r="R19">
+        <v>0.9495087526415451</v>
+      </c>
+      <c r="S19">
+        <v>0.9495087526415451</v>
+      </c>
+      <c r="T19">
+        <v>0.971292694172632</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20">
+      <c r="A20" s="1">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20">
+        <v>1.027173618904952</v>
+      </c>
+      <c r="D20">
+        <v>1.007149811752504</v>
+      </c>
+      <c r="E20">
+        <v>0.993448565442969</v>
+      </c>
+      <c r="F20">
+        <v>1.027173618904952</v>
+      </c>
+      <c r="G20">
+        <v>0.9949796103605618</v>
+      </c>
+      <c r="H20">
+        <v>1.007149811752504</v>
+      </c>
+      <c r="I20">
+        <v>0.9740750792802683</v>
+      </c>
+      <c r="J20">
+        <v>1.029531886213101</v>
+      </c>
+      <c r="K20">
+        <v>1.007149811752504</v>
+      </c>
+      <c r="L20">
+        <v>0.993448565442969</v>
+      </c>
+      <c r="M20">
+        <v>1.01031109217396</v>
+      </c>
+      <c r="N20">
+        <v>1.01031109217396</v>
+      </c>
+      <c r="O20">
+        <v>0.9982324212093964</v>
+      </c>
+      <c r="P20">
+        <v>1.009257332033475</v>
+      </c>
+      <c r="Q20">
+        <v>1.009257332033475</v>
+      </c>
+      <c r="R20">
+        <v>1.008730451963232</v>
+      </c>
+      <c r="S20">
+        <v>1.008730451963232</v>
+      </c>
+      <c r="T20">
+        <v>1.004393095325726</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20">
+      <c r="A21" s="1">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21">
+        <v>0.9722130771406368</v>
+      </c>
+      <c r="D21">
+        <v>1.142308003872336</v>
+      </c>
+      <c r="E21">
+        <v>0.9856795263322912</v>
+      </c>
+      <c r="F21">
+        <v>0.9722130771406368</v>
+      </c>
+      <c r="G21">
+        <v>1.007890703643511</v>
+      </c>
+      <c r="H21">
+        <v>1.142308003872336</v>
+      </c>
+      <c r="I21">
+        <v>0.9623569163748993</v>
+      </c>
+      <c r="J21">
+        <v>1.02187662150615</v>
+      </c>
+      <c r="K21">
+        <v>1.142308003872336</v>
+      </c>
+      <c r="L21">
+        <v>0.9856795263322912</v>
+      </c>
+      <c r="M21">
+        <v>0.9789463017364639</v>
+      </c>
+      <c r="N21">
+        <v>0.9789463017364639</v>
+      </c>
+      <c r="O21">
+        <v>0.9734165066159424</v>
+      </c>
+      <c r="P21">
+        <v>1.033400202448421</v>
+      </c>
+      <c r="Q21">
+        <v>1.033400202448421</v>
+      </c>
+      <c r="R21">
+        <v>1.0606271528044</v>
+      </c>
+      <c r="S21">
+        <v>1.0606271528044</v>
+      </c>
+      <c r="T21">
+        <v>1.015387474811637</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20">
+      <c r="A22" s="1">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22">
+        <v>1.457039515344589</v>
+      </c>
+      <c r="D22">
+        <v>2.392977173124855</v>
+      </c>
+      <c r="E22">
+        <v>0.9010736078904356</v>
+      </c>
+      <c r="F22">
+        <v>1.457039515344589</v>
+      </c>
+      <c r="G22">
+        <v>1.237954003213172</v>
+      </c>
+      <c r="H22">
+        <v>2.392977173124855</v>
+      </c>
+      <c r="I22">
+        <v>0.9293525787020379</v>
+      </c>
+      <c r="J22">
+        <v>0.9287588546661951</v>
+      </c>
+      <c r="K22">
+        <v>2.392977173124855</v>
+      </c>
+      <c r="L22">
+        <v>0.9010736078904356</v>
+      </c>
+      <c r="M22">
+        <v>1.179056561617512</v>
+      </c>
+      <c r="N22">
+        <v>1.179056561617512</v>
+      </c>
+      <c r="O22">
+        <v>1.095821900645688</v>
+      </c>
+      <c r="P22">
+        <v>1.583696765453293</v>
+      </c>
+      <c r="Q22">
+        <v>1.583696765453293</v>
+      </c>
+      <c r="R22">
+        <v>1.786016867371184</v>
+      </c>
+      <c r="S22">
+        <v>1.786016867371184</v>
+      </c>
+      <c r="T22">
+        <v>1.307859288823547</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20">
+      <c r="A23" s="1">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23">
+        <v>0.1205010798110092</v>
+      </c>
+      <c r="D23">
         <v>0.2206763046780738</v>
       </c>
-      <c r="D19">
+      <c r="E23">
+        <v>1.422359093028812</v>
+      </c>
+      <c r="F23">
         <v>0.1205010798110092</v>
       </c>
-      <c r="E19">
+      <c r="G23">
+        <v>1.347545454211956</v>
+      </c>
+      <c r="H23">
+        <v>0.2206763046780738</v>
+      </c>
+      <c r="I23">
+        <v>0.9842298711400587</v>
+      </c>
+      <c r="J23">
+        <v>1.155243654984034</v>
+      </c>
+      <c r="K23">
+        <v>0.2206763046780738</v>
+      </c>
+      <c r="L23">
         <v>1.422359093028812</v>
       </c>
-      <c r="F19">
-        <v>0.2206763046780738</v>
-      </c>
-      <c r="G19">
-        <v>1.155243654984034</v>
-      </c>
-      <c r="H19">
-        <v>0.9842298711400587</v>
-      </c>
-      <c r="I19">
-        <v>1.347545454211956</v>
-      </c>
-      <c r="J19">
-        <v>0.1205010798110092</v>
-      </c>
-      <c r="K19">
-        <v>0.2206763046780738</v>
-      </c>
-      <c r="L19">
-        <v>1.422359093028812</v>
-      </c>
-      <c r="M19">
+      <c r="M23">
         <v>0.7714300864199107</v>
       </c>
-      <c r="N19">
+      <c r="N23">
         <v>0.7714300864199107</v>
       </c>
-      <c r="O19">
+      <c r="O23">
         <v>0.8423633479932934</v>
       </c>
-      <c r="P19">
+      <c r="P23">
         <v>0.5878454925059651</v>
       </c>
-      <c r="Q19">
-        <v>0.5878454925059652</v>
-      </c>
-      <c r="R19">
-        <v>0.4960531955489923</v>
-      </c>
-      <c r="S19">
-        <v>0.4960531955489923</v>
-      </c>
-      <c r="T19">
+      <c r="Q23">
+        <v>0.5878454925059651</v>
+      </c>
+      <c r="R23">
+        <v>0.4960531955489922</v>
+      </c>
+      <c r="S23">
+        <v>0.4960531955489922</v>
+      </c>
+      <c r="T23">
         <v>0.8750925763089907</v>
       </c>
     </row>

</xml_diff>

<commit_message>
New simulation files for schemes report
</commit_message>
<xml_diff>
--- a/JupyterNotebooks/AvgHW/Alpha1F-HW03.xlsx
+++ b/JupyterNotebooks/AvgHW/Alpha1F-HW03.xlsx
@@ -14,36 +14,69 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>HKL</t>
   </si>
   <si>
-    <t>BT8Hex_2.5</t>
-  </si>
-  <si>
-    <t>BT8Hex_5</t>
-  </si>
-  <si>
-    <t>BT8Hex_10</t>
-  </si>
-  <si>
-    <t>BT8Hex_15</t>
-  </si>
-  <si>
-    <t>Spiral2.5</t>
-  </si>
-  <si>
     <t>Spiral5</t>
   </si>
   <si>
-    <t>Spiral7.5</t>
-  </si>
-  <si>
-    <t>Spiral10</t>
-  </si>
-  <si>
-    <t>Spiral15</t>
+    <t>RotRing OmegaMax-90</t>
+  </si>
+  <si>
+    <t>Equal Angle</t>
+  </si>
+  <si>
+    <t>Tilt Rotate</t>
+  </si>
+  <si>
+    <t>CLR</t>
+  </si>
+  <si>
+    <t>Rizzie Hex</t>
+  </si>
+  <si>
+    <t>Thomas Hex</t>
+  </si>
+  <si>
+    <t>Tilt Rotate_Partial</t>
+  </si>
+  <si>
+    <t>RotRing OmegaMax-60</t>
+  </si>
+  <si>
+    <t>Equal Angle_Partial</t>
+  </si>
+  <si>
+    <t>Rizzie Hex_Partial</t>
+  </si>
+  <si>
+    <t>ND Single</t>
+  </si>
+  <si>
+    <t>RD Single</t>
+  </si>
+  <si>
+    <t>TD Single</t>
+  </si>
+  <si>
+    <t>Morris Single</t>
+  </si>
+  <si>
+    <t>Ring Perpendicular to ND</t>
+  </si>
+  <si>
+    <t>Ring Perpendicular to RD</t>
+  </si>
+  <si>
+    <t>Ring Perpendicular to TD</t>
+  </si>
+  <si>
+    <t>OffsetFTD</t>
+  </si>
+  <si>
+    <t>OffsetATD</t>
   </si>
   <si>
     <t>OffsetF45</t>
@@ -52,46 +85,43 @@
     <t>OffsetA45</t>
   </si>
   <si>
-    <t>OffsetFTD</t>
-  </si>
-  <si>
-    <t>OffsetATD</t>
-  </si>
-  <si>
-    <t>HexGrid-90degTilt2.5degRes</t>
-  </si>
-  <si>
-    <t>HexGrid-90degTilt5degRes</t>
-  </si>
-  <si>
-    <t>HexGrid-90degTilt10degRes</t>
-  </si>
-  <si>
-    <t>HexGrid-90degTilt15degRes</t>
+    <t>OffsetFRD</t>
+  </si>
+  <si>
+    <t>OffsetARD</t>
+  </si>
+  <si>
+    <t>Gaussian Quadrature</t>
+  </si>
+  <si>
+    <t>Michael-CCHex</t>
+  </si>
+  <si>
+    <t>Michael-SNHex</t>
+  </si>
+  <si>
+    <t>[2, 0, 0]</t>
+  </si>
+  <si>
+    <t>[2, 2, 0]</t>
+  </si>
+  <si>
+    <t>[2, 1, 1]</t>
+  </si>
+  <si>
+    <t>[4, 0, 0]</t>
+  </si>
+  <si>
+    <t>[3, 2, 1]</t>
   </si>
   <si>
     <t>[1, 1, 0]</t>
   </si>
   <si>
-    <t>[2, 0, 0]</t>
-  </si>
-  <si>
-    <t>[2, 1, 1]</t>
-  </si>
-  <si>
-    <t>[2, 2, 0]</t>
+    <t>[3, 1, 0]</t>
   </si>
   <si>
     <t>[2, 2, 2]</t>
-  </si>
-  <si>
-    <t>[3, 1, 0]</t>
-  </si>
-  <si>
-    <t>[3, 2, 1]</t>
-  </si>
-  <si>
-    <t>[4, 0, 0]</t>
   </si>
   <si>
     <t>1Pair-A</t>
@@ -479,7 +509,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T19"/>
+  <dimension ref="A1:T29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -552,58 +582,58 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="E2" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="F2" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="G2" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="H2" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="I2" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="J2" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="K2" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="L2" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="M2" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="N2" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="O2" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="P2" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="Q2" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="R2" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="S2" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="T2" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:20">
@@ -614,58 +644,58 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>1.152945834855813</v>
+        <v>1.034234591157339</v>
       </c>
       <c r="D3">
-        <v>0.9536650201154075</v>
+        <v>1.091641707993742</v>
       </c>
       <c r="E3">
-        <v>0.937182945962484</v>
+        <v>0.9869027133780399</v>
       </c>
       <c r="F3">
-        <v>1.152945834855813</v>
+        <v>1.034234591157339</v>
       </c>
       <c r="G3">
-        <v>0.9432975636099349</v>
+        <v>0.9874922857148483</v>
       </c>
       <c r="H3">
-        <v>0.9422994293293789</v>
+        <v>1.091641707993742</v>
       </c>
       <c r="I3">
-        <v>1.041997125837943</v>
+        <v>0.9740675218658092</v>
       </c>
       <c r="J3">
-        <v>0.9536650201154075</v>
+        <v>1.022593623954924</v>
       </c>
       <c r="K3">
-        <v>1.152945834855813</v>
+        <v>1.091641707993742</v>
       </c>
       <c r="L3">
-        <v>0.937182945962484</v>
+        <v>0.9869027133780399</v>
       </c>
       <c r="M3">
-        <v>0.9454239830389457</v>
+        <v>1.010568652267689</v>
       </c>
       <c r="N3">
-        <v>0.9454239830389457</v>
+        <v>1.010568652267689</v>
       </c>
       <c r="O3">
-        <v>0.9443824651357567</v>
+        <v>0.9984016088003959</v>
       </c>
       <c r="P3">
-        <v>1.014597933644568</v>
+        <v>1.037593004176374</v>
       </c>
       <c r="Q3">
-        <v>1.014597933644568</v>
+        <v>1.037593004176374</v>
       </c>
       <c r="R3">
-        <v>1.049184908947379</v>
+        <v>1.051105180130716</v>
       </c>
       <c r="S3">
-        <v>1.049184908947379</v>
+        <v>1.051105180130716</v>
       </c>
       <c r="T3">
-        <v>0.9952313199518269</v>
+        <v>1.016155407344117</v>
       </c>
     </row>
     <row r="4" spans="1:20">
@@ -676,58 +706,58 @@
         <v>2</v>
       </c>
       <c r="C4">
-        <v>1.291315184167343</v>
+        <v>0.8845247616729527</v>
       </c>
       <c r="D4">
-        <v>1.225419474706893</v>
+        <v>1.082906649380325</v>
       </c>
       <c r="E4">
-        <v>0.9281919766583274</v>
+        <v>0.9551386270794382</v>
       </c>
       <c r="F4">
-        <v>1.291315184167343</v>
+        <v>0.8845247616729527</v>
       </c>
       <c r="G4">
-        <v>1.008385953488546</v>
+        <v>1.047394633441321</v>
       </c>
       <c r="H4">
-        <v>0.7039957044935053</v>
+        <v>1.082906649380325</v>
       </c>
       <c r="I4">
-        <v>1.143606536477421</v>
+        <v>0.7872592349169611</v>
       </c>
       <c r="J4">
-        <v>1.225419474706893</v>
+        <v>1.132495973221657</v>
       </c>
       <c r="K4">
-        <v>1.291315184167343</v>
+        <v>1.082906649380325</v>
       </c>
       <c r="L4">
-        <v>0.9281919766583274</v>
+        <v>0.9551386270794382</v>
       </c>
       <c r="M4">
-        <v>1.07680572568261</v>
+        <v>0.9198316943761955</v>
       </c>
       <c r="N4">
-        <v>1.07680572568261</v>
+        <v>0.9198316943761955</v>
       </c>
       <c r="O4">
-        <v>0.9525357186195751</v>
+        <v>0.8756408745564507</v>
       </c>
       <c r="P4">
-        <v>1.148308878510854</v>
+        <v>0.9741900127109052</v>
       </c>
       <c r="Q4">
-        <v>1.148308878510854</v>
+        <v>0.974190012710905</v>
       </c>
       <c r="R4">
-        <v>1.184060454924976</v>
+        <v>1.00136917187826</v>
       </c>
       <c r="S4">
-        <v>1.184060454924976</v>
+        <v>1.00136917187826</v>
       </c>
       <c r="T4">
-        <v>1.050152471665339</v>
+        <v>0.981619979952109</v>
       </c>
     </row>
     <row r="5" spans="1:20">
@@ -738,58 +768,58 @@
         <v>3</v>
       </c>
       <c r="C5">
-        <v>2.051584262501862</v>
+        <v>1.173761791692285</v>
       </c>
       <c r="D5">
-        <v>0.1288273206544606</v>
+        <v>0.9988664757047482</v>
       </c>
       <c r="E5">
-        <v>0.9885706214910599</v>
+        <v>0.8143293733694247</v>
       </c>
       <c r="F5">
-        <v>2.051584262501862</v>
+        <v>1.173761791692285</v>
       </c>
       <c r="G5">
-        <v>0.6813256377537013</v>
+        <v>0.8630531185074014</v>
       </c>
       <c r="H5">
-        <v>0.6793054559236139</v>
+        <v>0.9988664757047482</v>
       </c>
       <c r="I5">
-        <v>1.664477351232213</v>
+        <v>1.040072132954511</v>
       </c>
       <c r="J5">
-        <v>0.1288273206544606</v>
+        <v>0.7708217850544109</v>
       </c>
       <c r="K5">
-        <v>2.051584262501862</v>
+        <v>0.9988664757047482</v>
       </c>
       <c r="L5">
-        <v>0.9885706214910599</v>
+        <v>0.8143293733694247</v>
       </c>
       <c r="M5">
-        <v>0.5586989710727602</v>
+        <v>0.9940455825308547</v>
       </c>
       <c r="N5">
-        <v>0.5586989710727602</v>
+        <v>0.9940455825308547</v>
       </c>
       <c r="O5">
-        <v>0.5989011326897115</v>
+        <v>1.009387766005407</v>
       </c>
       <c r="P5">
-        <v>1.056327401549128</v>
+        <v>0.9956525469221525</v>
       </c>
       <c r="Q5">
-        <v>1.056327401549128</v>
+        <v>0.9956525469221525</v>
       </c>
       <c r="R5">
-        <v>1.305141616787311</v>
+        <v>0.9964560291178014</v>
       </c>
       <c r="S5">
-        <v>1.305141616787311</v>
+        <v>0.9964560291178014</v>
       </c>
       <c r="T5">
-        <v>1.032348441592818</v>
+        <v>0.9434841128804634</v>
       </c>
     </row>
     <row r="6" spans="1:20">
@@ -800,58 +830,58 @@
         <v>4</v>
       </c>
       <c r="C6">
-        <v>4.218585539063117</v>
+        <v>0.5787035104381049</v>
       </c>
       <c r="D6">
-        <v>-0.00018860899178274</v>
+        <v>0.4662126205697955</v>
       </c>
       <c r="E6">
-        <v>0.03829107386291899</v>
+        <v>0.4591235400880798</v>
       </c>
       <c r="F6">
-        <v>4.218585539063117</v>
+        <v>0.5787035104381049</v>
       </c>
       <c r="G6">
-        <v>1.903788088321897</v>
+        <v>0.436242668215461</v>
       </c>
       <c r="H6">
-        <v>0.5955406690348662</v>
+        <v>0.4662126205697955</v>
       </c>
       <c r="I6">
-        <v>1.343956095415291</v>
+        <v>0.5441068785151475</v>
       </c>
       <c r="J6">
-        <v>-0.00018860899178274</v>
+        <v>0.4232749538598622</v>
       </c>
       <c r="K6">
-        <v>4.218585539063117</v>
+        <v>0.4662126205697955</v>
       </c>
       <c r="L6">
-        <v>0.03829107386291899</v>
+        <v>0.4591235400880798</v>
       </c>
       <c r="M6">
-        <v>0.01905123243556812</v>
+        <v>0.5189135252630923</v>
       </c>
       <c r="N6">
-        <v>0.01905123243556812</v>
+        <v>0.5189135252630923</v>
       </c>
       <c r="O6">
-        <v>0.2112143779686675</v>
+        <v>0.527311309680444</v>
       </c>
       <c r="P6">
-        <v>1.418896001311418</v>
+        <v>0.5013465570319934</v>
       </c>
       <c r="Q6">
-        <v>1.418896001311418</v>
+        <v>0.5013465570319934</v>
       </c>
       <c r="R6">
-        <v>2.118818385749343</v>
+        <v>0.4925630729164439</v>
       </c>
       <c r="S6">
-        <v>2.118818385749343</v>
+        <v>0.4925630729164439</v>
       </c>
       <c r="T6">
-        <v>1.349995476117718</v>
+        <v>0.4846106952810751</v>
       </c>
     </row>
     <row r="7" spans="1:20">
@@ -862,58 +892,58 @@
         <v>5</v>
       </c>
       <c r="C7">
-        <v>1.047986879235474</v>
+        <v>0.9846422066275502</v>
       </c>
       <c r="D7">
-        <v>1.01995925681131</v>
+        <v>1.146734370382373</v>
       </c>
       <c r="E7">
-        <v>0.9918784523322198</v>
+        <v>0.9237831735460421</v>
       </c>
       <c r="F7">
-        <v>1.047986879235474</v>
+        <v>0.9846422066275502</v>
       </c>
       <c r="G7">
-        <v>1.024127889905488</v>
+        <v>1.054145349892974</v>
       </c>
       <c r="H7">
-        <v>0.9739851518986554</v>
+        <v>1.146734370382373</v>
       </c>
       <c r="I7">
-        <v>0.9925111675685035</v>
+        <v>0.9458238522669338</v>
       </c>
       <c r="J7">
-        <v>1.01995925681131</v>
+        <v>0.9646010997971536</v>
       </c>
       <c r="K7">
-        <v>1.047986879235474</v>
+        <v>1.146734370382373</v>
       </c>
       <c r="L7">
-        <v>0.9918784523322198</v>
+        <v>0.9237831735460421</v>
       </c>
       <c r="M7">
-        <v>1.005918854571765</v>
+        <v>0.9542126900867962</v>
       </c>
       <c r="N7">
-        <v>1.005918854571765</v>
+        <v>0.9542126900867962</v>
       </c>
       <c r="O7">
-        <v>0.9952742870140616</v>
+        <v>0.9514164108135087</v>
       </c>
       <c r="P7">
-        <v>1.019941529459668</v>
+        <v>1.018386583518655</v>
       </c>
       <c r="Q7">
-        <v>1.019941529459668</v>
+        <v>1.018386583518655</v>
       </c>
       <c r="R7">
-        <v>1.026952866903619</v>
+        <v>1.050473530234584</v>
       </c>
       <c r="S7">
-        <v>1.026952866903619</v>
+        <v>1.050473530234584</v>
       </c>
       <c r="T7">
-        <v>1.008408132958609</v>
+        <v>1.003288342085504</v>
       </c>
     </row>
     <row r="8" spans="1:20">
@@ -924,58 +954,58 @@
         <v>6</v>
       </c>
       <c r="C8">
-        <v>1.091641707993743</v>
+        <v>0.9722130771406368</v>
       </c>
       <c r="D8">
-        <v>1.034234591157332</v>
+        <v>1.142308003872336</v>
       </c>
       <c r="E8">
-        <v>0.98690271337804</v>
+        <v>0.9856795263322912</v>
       </c>
       <c r="F8">
-        <v>1.091641707993743</v>
+        <v>0.9722130771406368</v>
       </c>
       <c r="G8">
-        <v>1.022593623954923</v>
+        <v>1.007890703643511</v>
       </c>
       <c r="H8">
-        <v>0.9740675218658092</v>
+        <v>1.142308003872336</v>
       </c>
       <c r="I8">
-        <v>0.9874922857148486</v>
+        <v>0.9623569163748993</v>
       </c>
       <c r="J8">
-        <v>1.034234591157332</v>
+        <v>1.02187662150615</v>
       </c>
       <c r="K8">
-        <v>1.091641707993743</v>
+        <v>1.142308003872336</v>
       </c>
       <c r="L8">
-        <v>0.98690271337804</v>
+        <v>0.9856795263322912</v>
       </c>
       <c r="M8">
-        <v>1.010568652267686</v>
+        <v>0.9789463017364639</v>
       </c>
       <c r="N8">
-        <v>1.010568652267686</v>
+        <v>0.9789463017364639</v>
       </c>
       <c r="O8">
-        <v>0.9984016088003939</v>
+        <v>0.9734165066159424</v>
       </c>
       <c r="P8">
-        <v>1.037593004176372</v>
+        <v>1.033400202448421</v>
       </c>
       <c r="Q8">
-        <v>1.037593004176372</v>
+        <v>1.033400202448421</v>
       </c>
       <c r="R8">
-        <v>1.051105180130715</v>
+        <v>1.0606271528044</v>
       </c>
       <c r="S8">
-        <v>1.051105180130715</v>
+        <v>1.0606271528044</v>
       </c>
       <c r="T8">
-        <v>1.016155407344116</v>
+        <v>1.015387474811637</v>
       </c>
     </row>
     <row r="9" spans="1:20">
@@ -986,58 +1016,58 @@
         <v>7</v>
       </c>
       <c r="C9">
-        <v>1.258806238220695</v>
+        <v>1.225419474706893</v>
       </c>
       <c r="D9">
-        <v>0.9675462776458512</v>
+        <v>1.291315184167343</v>
       </c>
       <c r="E9">
-        <v>0.9693562270106392</v>
+        <v>0.9281919766583274</v>
       </c>
       <c r="F9">
-        <v>1.258806238220695</v>
+        <v>1.225419474706893</v>
       </c>
       <c r="G9">
-        <v>0.9783919335572949</v>
+        <v>1.143606536477421</v>
       </c>
       <c r="H9">
-        <v>0.9603048457350024</v>
+        <v>1.291315184167343</v>
       </c>
       <c r="I9">
-        <v>0.9729641384379286</v>
+        <v>0.7039957044935053</v>
       </c>
       <c r="J9">
-        <v>0.9675462776458512</v>
+        <v>1.008385953488546</v>
       </c>
       <c r="K9">
-        <v>1.258806238220695</v>
+        <v>1.291315184167343</v>
       </c>
       <c r="L9">
-        <v>0.9693562270106392</v>
+        <v>0.9281919766583274</v>
       </c>
       <c r="M9">
-        <v>0.9684512523282451</v>
+        <v>1.07680572568261</v>
       </c>
       <c r="N9">
-        <v>0.9684512523282451</v>
+        <v>1.07680572568261</v>
       </c>
       <c r="O9">
-        <v>0.9657357834638308</v>
+        <v>0.9525357186195751</v>
       </c>
       <c r="P9">
-        <v>1.065236247625728</v>
+        <v>1.148308878510854</v>
       </c>
       <c r="Q9">
-        <v>1.065236247625728</v>
+        <v>1.148308878510854</v>
       </c>
       <c r="R9">
-        <v>1.11362874527447</v>
+        <v>1.184060454924976</v>
       </c>
       <c r="S9">
-        <v>1.11362874527447</v>
+        <v>1.184060454924976</v>
       </c>
       <c r="T9">
-        <v>1.017894943434569</v>
+        <v>1.050152471665339</v>
       </c>
     </row>
     <row r="10" spans="1:20">
@@ -1048,58 +1078,58 @@
         <v>8</v>
       </c>
       <c r="C10">
-        <v>1.534687420495374</v>
+        <v>0.6069740241260413</v>
       </c>
       <c r="D10">
-        <v>1.018142314512956</v>
+        <v>0.4421357857954734</v>
       </c>
       <c r="E10">
-        <v>1.062993573522152</v>
+        <v>0.4273157588461299</v>
       </c>
       <c r="F10">
-        <v>1.534687420495374</v>
+        <v>0.6069740241260413</v>
       </c>
       <c r="G10">
-        <v>1.110109093028632</v>
+        <v>0.4167866881363111</v>
       </c>
       <c r="H10">
-        <v>0.8590858623377114</v>
+        <v>0.4421357857954734</v>
       </c>
       <c r="I10">
-        <v>1.063100811713334</v>
+        <v>0.5485888796317363</v>
       </c>
       <c r="J10">
-        <v>1.018142314512956</v>
+        <v>0.4595612543949866</v>
       </c>
       <c r="K10">
-        <v>1.534687420495374</v>
+        <v>0.4421357857954734</v>
       </c>
       <c r="L10">
-        <v>1.062993573522152</v>
+        <v>0.4273157588461299</v>
       </c>
       <c r="M10">
-        <v>1.040567944017554</v>
+        <v>0.5171448914860856</v>
       </c>
       <c r="N10">
-        <v>1.040567944017554</v>
+        <v>0.5171448914860856</v>
       </c>
       <c r="O10">
-        <v>0.9800739167909399</v>
+        <v>0.5276262208679691</v>
       </c>
       <c r="P10">
-        <v>1.205274436176827</v>
+        <v>0.4921418562558815</v>
       </c>
       <c r="Q10">
-        <v>1.205274436176827</v>
+        <v>0.4921418562558815</v>
       </c>
       <c r="R10">
-        <v>1.287627682256464</v>
+        <v>0.4796403386407794</v>
       </c>
       <c r="S10">
-        <v>1.287627682256464</v>
+        <v>0.4796403386407794</v>
       </c>
       <c r="T10">
-        <v>1.108019845935027</v>
+        <v>0.4835603984884465</v>
       </c>
     </row>
     <row r="11" spans="1:20">
@@ -1110,58 +1140,58 @@
         <v>9</v>
       </c>
       <c r="C11">
-        <v>2.333464727294784</v>
+        <v>0.8723211855978082</v>
       </c>
       <c r="D11">
-        <v>1.199301118019966</v>
+        <v>0.8611351388353655</v>
       </c>
       <c r="E11">
-        <v>0.8213258604366268</v>
+        <v>0.9851915386376003</v>
       </c>
       <c r="F11">
-        <v>2.333464727294784</v>
+        <v>0.8723211855978082</v>
       </c>
       <c r="G11">
-        <v>0.6087295150139962</v>
+        <v>1.19771356375457</v>
       </c>
       <c r="H11">
-        <v>0.8342399679404157</v>
+        <v>0.8611351388353655</v>
       </c>
       <c r="I11">
-        <v>0.9523004446201929</v>
+        <v>0.8543971311857294</v>
       </c>
       <c r="J11">
-        <v>1.199301118019966</v>
+        <v>0.4570903765846644</v>
       </c>
       <c r="K11">
-        <v>2.333464727294784</v>
+        <v>0.8611351388353655</v>
       </c>
       <c r="L11">
-        <v>0.8213258604366268</v>
+        <v>0.9851915386376003</v>
       </c>
       <c r="M11">
-        <v>1.010313489228296</v>
+        <v>0.9287563621177043</v>
       </c>
       <c r="N11">
-        <v>1.010313489228296</v>
+        <v>0.9287563621177043</v>
       </c>
       <c r="O11">
-        <v>0.9516223154656694</v>
+        <v>0.903969951807046</v>
       </c>
       <c r="P11">
-        <v>1.451363901917126</v>
+        <v>0.9062159543569247</v>
       </c>
       <c r="Q11">
-        <v>1.451363901917126</v>
+        <v>0.9062159543569247</v>
       </c>
       <c r="R11">
-        <v>1.67188910826154</v>
+        <v>0.8949457504765349</v>
       </c>
       <c r="S11">
-        <v>1.67188910826154</v>
+        <v>0.8949457504765349</v>
       </c>
       <c r="T11">
-        <v>1.12489360555433</v>
+        <v>0.8713081557659564</v>
       </c>
     </row>
     <row r="12" spans="1:20">
@@ -1172,58 +1202,58 @@
         <v>10</v>
       </c>
       <c r="C12">
-        <v>1.650333686930785</v>
+        <v>1.11308471458956</v>
       </c>
       <c r="D12">
-        <v>0.0009906382284935974</v>
+        <v>0.8571234646570741</v>
       </c>
       <c r="E12">
-        <v>0.9268749225926884</v>
+        <v>0.8428092352636376</v>
       </c>
       <c r="F12">
-        <v>1.650333686930785</v>
+        <v>1.11308471458956</v>
       </c>
       <c r="G12">
-        <v>0.001147664018377606</v>
+        <v>0.8127840244326886</v>
       </c>
       <c r="H12">
-        <v>1.891613563536644</v>
+        <v>0.8571234646570741</v>
       </c>
       <c r="I12">
-        <v>2.223509045495451</v>
+        <v>1.073065520892483</v>
       </c>
       <c r="J12">
-        <v>0.0009906382284935974</v>
+        <v>0.876702440456508</v>
       </c>
       <c r="K12">
-        <v>1.650333686930785</v>
+        <v>0.8571234646570741</v>
       </c>
       <c r="L12">
-        <v>0.9268749225926884</v>
+        <v>0.8428092352636376</v>
       </c>
       <c r="M12">
-        <v>0.463932780410591</v>
+        <v>0.9779469749265987</v>
       </c>
       <c r="N12">
-        <v>0.463932780410591</v>
+        <v>0.9779469749265987</v>
       </c>
       <c r="O12">
-        <v>0.9398263747859422</v>
+        <v>1.009653156915227</v>
       </c>
       <c r="P12">
-        <v>0.8593997492506555</v>
+        <v>0.9376724715034238</v>
       </c>
       <c r="Q12">
-        <v>0.8593997492506557</v>
+        <v>0.9376724715034239</v>
       </c>
       <c r="R12">
-        <v>1.057133233670688</v>
+        <v>0.9175352197918365</v>
       </c>
       <c r="S12">
-        <v>1.057133233670688</v>
+        <v>0.9175352197918365</v>
       </c>
       <c r="T12">
-        <v>1.11574492013374</v>
+        <v>0.9292615667153252</v>
       </c>
     </row>
     <row r="13" spans="1:20">
@@ -1234,58 +1264,58 @@
         <v>11</v>
       </c>
       <c r="C13">
-        <v>0.7953816718760839</v>
+        <v>0.6699817763633297</v>
       </c>
       <c r="D13">
-        <v>3.806806310651665</v>
+        <v>1.271008044503521</v>
       </c>
       <c r="E13">
-        <v>1.257223936975513</v>
+        <v>1.115278358379869</v>
       </c>
       <c r="F13">
-        <v>0.7953816718760839</v>
+        <v>0.6699817763633297</v>
       </c>
       <c r="G13">
-        <v>2.492586044649236</v>
+        <v>1.087123251781193</v>
       </c>
       <c r="H13">
-        <v>1.878161985072148</v>
+        <v>1.271008044503521</v>
       </c>
       <c r="I13">
-        <v>1.380876313850262</v>
+        <v>0.7746128494181943</v>
       </c>
       <c r="J13">
-        <v>3.806806310651665</v>
+        <v>1.410886158389823</v>
       </c>
       <c r="K13">
-        <v>0.7953816718760839</v>
+        <v>1.271008044503521</v>
       </c>
       <c r="L13">
-        <v>1.257223936975513</v>
+        <v>1.115278358379869</v>
       </c>
       <c r="M13">
-        <v>2.532015123813589</v>
+        <v>0.8926300673715994</v>
       </c>
       <c r="N13">
-        <v>2.532015123813589</v>
+        <v>0.8926300673715994</v>
       </c>
       <c r="O13">
-        <v>2.314064077566442</v>
+        <v>0.8532909947204644</v>
       </c>
       <c r="P13">
-        <v>1.953137306501087</v>
+        <v>1.018756059748907</v>
       </c>
       <c r="Q13">
-        <v>1.953137306501087</v>
+        <v>1.018756059748907</v>
       </c>
       <c r="R13">
-        <v>1.663698397844836</v>
+        <v>1.08181905593756</v>
       </c>
       <c r="S13">
-        <v>1.663698397844836</v>
+        <v>1.08181905593756</v>
       </c>
       <c r="T13">
-        <v>1.935172710512485</v>
+        <v>1.054815073139322</v>
       </c>
     </row>
     <row r="14" spans="1:20">
@@ -1296,58 +1326,58 @@
         <v>12</v>
       </c>
       <c r="C14">
-        <v>-0.0007584295794183397</v>
+        <v>-0.01248147300000001</v>
       </c>
       <c r="D14">
-        <v>0.549028529025309</v>
+        <v>-0.0009139994799999984</v>
       </c>
       <c r="E14">
-        <v>1.694874496173249</v>
+        <v>-0.010207482</v>
       </c>
       <c r="F14">
-        <v>-0.0007584295794183397</v>
+        <v>-0.01248147300000001</v>
       </c>
       <c r="G14">
-        <v>0.07992494560801593</v>
+        <v>0.005017741899999998</v>
       </c>
       <c r="H14">
-        <v>2.163906465814728</v>
+        <v>-0.0009139994799999984</v>
       </c>
       <c r="I14">
-        <v>0.09679846039972904</v>
+        <v>0.024963772</v>
       </c>
       <c r="J14">
-        <v>0.549028529025309</v>
+        <v>0.004912388499999995</v>
       </c>
       <c r="K14">
-        <v>-0.0007584295794183397</v>
+        <v>-0.0009139994799999984</v>
       </c>
       <c r="L14">
-        <v>1.694874496173249</v>
+        <v>-0.010207482</v>
       </c>
       <c r="M14">
-        <v>1.121951512599279</v>
+        <v>-0.01134447750000001</v>
       </c>
       <c r="N14">
-        <v>1.121951512599279</v>
+        <v>-0.01134447750000001</v>
       </c>
       <c r="O14">
-        <v>1.469269830337762</v>
+        <v>0.0007582723333333293</v>
       </c>
       <c r="P14">
-        <v>0.74771486520638</v>
+        <v>-0.007867651493333336</v>
       </c>
       <c r="Q14">
-        <v>0.74771486520638</v>
+        <v>-0.007867651493333336</v>
       </c>
       <c r="R14">
-        <v>0.5605965415099303</v>
+        <v>-0.006129238490000001</v>
       </c>
       <c r="S14">
-        <v>0.5605965415099303</v>
+        <v>-0.006129238490000001</v>
       </c>
       <c r="T14">
-        <v>0.7639624112402689</v>
+        <v>0.001881824653333331</v>
       </c>
     </row>
     <row r="15" spans="1:20">
@@ -1358,58 +1388,58 @@
         <v>13</v>
       </c>
       <c r="C15">
-        <v>0.07529789264772961</v>
+        <v>0.00070900843</v>
       </c>
       <c r="D15">
-        <v>0.06949281876991974</v>
+        <v>121.14151</v>
       </c>
       <c r="E15">
-        <v>0.4828810263023473</v>
+        <v>-0.012240956</v>
       </c>
       <c r="F15">
-        <v>0.07529789264772961</v>
+        <v>0.00070900843</v>
       </c>
       <c r="G15">
-        <v>0.01587949993991768</v>
+        <v>-0.0067091534</v>
       </c>
       <c r="H15">
-        <v>-0.0004574272900550843</v>
+        <v>121.14151</v>
       </c>
       <c r="I15">
-        <v>1.401767971530122</v>
+        <v>-0.0017802751</v>
       </c>
       <c r="J15">
-        <v>0.06949281876991974</v>
+        <v>0.010282672</v>
       </c>
       <c r="K15">
-        <v>0.07529789264772961</v>
+        <v>121.14151</v>
       </c>
       <c r="L15">
-        <v>0.4828810263023473</v>
+        <v>-0.012240956</v>
       </c>
       <c r="M15">
-        <v>0.2761869225361335</v>
+        <v>-0.005765973785000001</v>
       </c>
       <c r="N15">
-        <v>0.2761869225361335</v>
+        <v>-0.005765973785000001</v>
       </c>
       <c r="O15">
-        <v>0.1839721392607373</v>
+        <v>-0.004437407556666668</v>
       </c>
       <c r="P15">
-        <v>0.2092239125733322</v>
+        <v>40.37665935080999</v>
       </c>
       <c r="Q15">
-        <v>0.2092239125733322</v>
+        <v>40.37665935080999</v>
       </c>
       <c r="R15">
-        <v>0.1757424075919315</v>
+        <v>60.5678720131075</v>
       </c>
       <c r="S15">
-        <v>0.1757424075919315</v>
+        <v>60.5678720131075</v>
       </c>
       <c r="T15">
-        <v>0.3408102969833302</v>
+        <v>20.18862854932167</v>
       </c>
     </row>
     <row r="16" spans="1:20">
@@ -1420,58 +1450,58 @@
         <v>14</v>
       </c>
       <c r="C16">
-        <v>1.007149811752503</v>
+        <v>0.016549232</v>
       </c>
       <c r="D16">
-        <v>1.027173618904952</v>
+        <v>-0.0025525058</v>
       </c>
       <c r="E16">
-        <v>0.9934485654429699</v>
+        <v>-0.010349456</v>
       </c>
       <c r="F16">
-        <v>1.007149811752503</v>
+        <v>0.016549232</v>
       </c>
       <c r="G16">
-        <v>1.029531886213101</v>
+        <v>-0.0019770734</v>
       </c>
       <c r="H16">
-        <v>0.9740750792802707</v>
+        <v>-0.0025525058</v>
       </c>
       <c r="I16">
-        <v>0.9949796103605598</v>
+        <v>-0.011953383</v>
       </c>
       <c r="J16">
-        <v>1.027173618904952</v>
+        <v>-0.017342988</v>
       </c>
       <c r="K16">
-        <v>1.007149811752503</v>
+        <v>-0.0025525058</v>
       </c>
       <c r="L16">
-        <v>0.9934485654429699</v>
+        <v>-0.010349456</v>
       </c>
       <c r="M16">
-        <v>1.010311092173961</v>
+        <v>0.003099888</v>
       </c>
       <c r="N16">
-        <v>1.010311092173961</v>
+        <v>0.003099888</v>
       </c>
       <c r="O16">
-        <v>0.9982324212093977</v>
+        <v>-0.001917869</v>
       </c>
       <c r="P16">
-        <v>1.009257332033475</v>
+        <v>0.001215756733333334</v>
       </c>
       <c r="Q16">
-        <v>1.009257332033475</v>
+        <v>0.001215756733333333</v>
       </c>
       <c r="R16">
-        <v>1.008730451963232</v>
+        <v>0.0002736911000000001</v>
       </c>
       <c r="S16">
-        <v>1.008730451963232</v>
+        <v>0.0002736911000000001</v>
       </c>
       <c r="T16">
-        <v>1.004393095325726</v>
+        <v>-0.004604362366666667</v>
       </c>
     </row>
     <row r="17" spans="1:20">
@@ -1482,58 +1512,58 @@
         <v>15</v>
       </c>
       <c r="C17">
-        <v>1.142308003872337</v>
+        <v>-0.00014894864</v>
       </c>
       <c r="D17">
-        <v>0.972213077140635</v>
+        <v>-0.0057702847</v>
       </c>
       <c r="E17">
-        <v>0.9856795263322907</v>
+        <v>0.0021540222</v>
       </c>
       <c r="F17">
-        <v>1.142308003872337</v>
+        <v>-0.00014894864</v>
       </c>
       <c r="G17">
-        <v>1.02187662150615</v>
+        <v>-0.0039257384</v>
       </c>
       <c r="H17">
-        <v>0.9623569163749013</v>
+        <v>-0.0057702847</v>
       </c>
       <c r="I17">
-        <v>1.007890703643512</v>
+        <v>0.00088323181</v>
       </c>
       <c r="J17">
-        <v>0.972213077140635</v>
+        <v>0.0043434522</v>
       </c>
       <c r="K17">
-        <v>1.142308003872337</v>
+        <v>-0.0057702847</v>
       </c>
       <c r="L17">
-        <v>0.9856795263322907</v>
+        <v>0.0021540222</v>
       </c>
       <c r="M17">
-        <v>0.9789463017364628</v>
+        <v>0.00100253678</v>
       </c>
       <c r="N17">
-        <v>0.9789463017364628</v>
+        <v>0.00100253678</v>
       </c>
       <c r="O17">
-        <v>0.9734165066159424</v>
+        <v>0.0009627684566666667</v>
       </c>
       <c r="P17">
-        <v>1.033400202448421</v>
+        <v>-0.00125507038</v>
       </c>
       <c r="Q17">
-        <v>1.033400202448421</v>
+        <v>-0.00125507038</v>
       </c>
       <c r="R17">
-        <v>1.0606271528044</v>
+        <v>-0.00238387396</v>
       </c>
       <c r="S17">
-        <v>1.0606271528044</v>
+        <v>-0.00238387396</v>
       </c>
       <c r="T17">
-        <v>1.015387474811638</v>
+        <v>-0.0004107109216666668</v>
       </c>
     </row>
     <row r="18" spans="1:20">
@@ -1544,58 +1574,58 @@
         <v>16</v>
       </c>
       <c r="C18">
-        <v>2.392977173124852</v>
+        <v>-0.005294425011917811</v>
       </c>
       <c r="D18">
-        <v>1.457039515344586</v>
+        <v>5.395919898593863</v>
       </c>
       <c r="E18">
-        <v>0.9010736078904343</v>
+        <v>0.0006851950339726029</v>
       </c>
       <c r="F18">
-        <v>2.392977173124852</v>
+        <v>-0.005294425011917811</v>
       </c>
       <c r="G18">
-        <v>0.9287588546661991</v>
+        <v>1.811715642742466</v>
       </c>
       <c r="H18">
-        <v>0.9293525787020404</v>
+        <v>5.395919898593863</v>
       </c>
       <c r="I18">
-        <v>1.23795400321317</v>
+        <v>0.02582977893013699</v>
       </c>
       <c r="J18">
-        <v>1.457039515344586</v>
+        <v>0.0003422312493150687</v>
       </c>
       <c r="K18">
-        <v>2.392977173124852</v>
+        <v>5.395919898593863</v>
       </c>
       <c r="L18">
-        <v>0.9010736078904343</v>
+        <v>0.0006851950339726029</v>
       </c>
       <c r="M18">
-        <v>1.17905656161751</v>
+        <v>-0.002304614988972604</v>
       </c>
       <c r="N18">
-        <v>1.17905656161751</v>
+        <v>-0.002304614988972604</v>
       </c>
       <c r="O18">
-        <v>1.095821900645687</v>
+        <v>0.00707351631739726</v>
       </c>
       <c r="P18">
-        <v>1.583696765453291</v>
+        <v>1.797103556205306</v>
       </c>
       <c r="Q18">
-        <v>1.583696765453291</v>
+        <v>1.797103556205306</v>
       </c>
       <c r="R18">
-        <v>1.786016867371181</v>
+        <v>2.696807641802445</v>
       </c>
       <c r="S18">
-        <v>1.786016867371181</v>
+        <v>2.696807641802445</v>
       </c>
       <c r="T18">
-        <v>1.307859288823547</v>
+        <v>1.204866386922973</v>
       </c>
     </row>
     <row r="19" spans="1:20">
@@ -1606,58 +1636,678 @@
         <v>17</v>
       </c>
       <c r="C19">
-        <v>0.2206763046780738</v>
+        <v>7.002471562811579</v>
       </c>
       <c r="D19">
-        <v>0.1205010798110092</v>
+        <v>3.501838080206315</v>
       </c>
       <c r="E19">
-        <v>1.422359093028812</v>
+        <v>3.496064890227895</v>
       </c>
       <c r="F19">
-        <v>0.2206763046780738</v>
+        <v>7.002471562811579</v>
       </c>
       <c r="G19">
-        <v>1.155243654984034</v>
+        <v>-0.005191953220894737</v>
       </c>
       <c r="H19">
-        <v>0.9842298711400587</v>
+        <v>3.501838080206315</v>
       </c>
       <c r="I19">
-        <v>1.347545454211956</v>
+        <v>0.001817788109157895</v>
       </c>
       <c r="J19">
-        <v>0.1205010798110092</v>
+        <v>10.48957806246842</v>
       </c>
       <c r="K19">
-        <v>0.2206763046780738</v>
+        <v>3.501838080206315</v>
       </c>
       <c r="L19">
-        <v>1.422359093028812</v>
+        <v>3.496064890227895</v>
       </c>
       <c r="M19">
-        <v>0.7714300864199107</v>
+        <v>5.249268226519737</v>
       </c>
       <c r="N19">
-        <v>0.7714300864199107</v>
+        <v>5.249268226519737</v>
       </c>
       <c r="O19">
-        <v>0.8423633479932934</v>
+        <v>3.500118080382877</v>
       </c>
       <c r="P19">
-        <v>0.5878454925059651</v>
+        <v>4.66679151108193</v>
       </c>
       <c r="Q19">
-        <v>0.5878454925059652</v>
+        <v>4.66679151108193</v>
       </c>
       <c r="R19">
-        <v>0.4960531955489923</v>
+        <v>4.375553153363026</v>
       </c>
       <c r="S19">
-        <v>0.4960531955489923</v>
+        <v>4.375553153363026</v>
       </c>
       <c r="T19">
-        <v>0.8750925763089907</v>
+        <v>4.081096405100413</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20">
+      <c r="A20" s="1">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20">
+        <v>0.001358614239473684</v>
+      </c>
+      <c r="D20">
+        <v>6.778065580148422</v>
+      </c>
+      <c r="E20">
+        <v>0.0009891908884210525</v>
+      </c>
+      <c r="F20">
+        <v>0.001358614239473684</v>
+      </c>
+      <c r="G20">
+        <v>1.124473584028421</v>
+      </c>
+      <c r="H20">
+        <v>6.778065580148422</v>
+      </c>
+      <c r="I20">
+        <v>1.647539540644316</v>
+      </c>
+      <c r="J20">
+        <v>0.01061339926157895</v>
+      </c>
+      <c r="K20">
+        <v>6.778065580148422</v>
+      </c>
+      <c r="L20">
+        <v>0.0009891908884210525</v>
+      </c>
+      <c r="M20">
+        <v>0.001173902563947368</v>
+      </c>
+      <c r="N20">
+        <v>0.001173902563947368</v>
+      </c>
+      <c r="O20">
+        <v>0.5499624485907368</v>
+      </c>
+      <c r="P20">
+        <v>2.260137795092105</v>
+      </c>
+      <c r="Q20">
+        <v>2.260137795092105</v>
+      </c>
+      <c r="R20">
+        <v>3.389619741356184</v>
+      </c>
+      <c r="S20">
+        <v>3.389619741356184</v>
+      </c>
+      <c r="T20">
+        <v>1.593839984868439</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20">
+      <c r="A21" s="1">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21">
+        <v>0.5490285290253076</v>
+      </c>
+      <c r="D21">
+        <v>-0.000758429579418342</v>
+      </c>
+      <c r="E21">
+        <v>1.694874496173247</v>
+      </c>
+      <c r="F21">
+        <v>0.5490285290253076</v>
+      </c>
+      <c r="G21">
+        <v>0.09679846039972893</v>
+      </c>
+      <c r="H21">
+        <v>-0.000758429579418342</v>
+      </c>
+      <c r="I21">
+        <v>2.163906465814728</v>
+      </c>
+      <c r="J21">
+        <v>0.07992494560801601</v>
+      </c>
+      <c r="K21">
+        <v>-0.000758429579418342</v>
+      </c>
+      <c r="L21">
+        <v>1.694874496173247</v>
+      </c>
+      <c r="M21">
+        <v>1.121951512599277</v>
+      </c>
+      <c r="N21">
+        <v>1.121951512599277</v>
+      </c>
+      <c r="O21">
+        <v>1.469269830337761</v>
+      </c>
+      <c r="P21">
+        <v>0.7477148652063786</v>
+      </c>
+      <c r="Q21">
+        <v>0.7477148652063788</v>
+      </c>
+      <c r="R21">
+        <v>0.5605965415099294</v>
+      </c>
+      <c r="S21">
+        <v>0.5605965415099294</v>
+      </c>
+      <c r="T21">
+        <v>0.763962411240268</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20">
+      <c r="A22" s="1">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22">
+        <v>0.06949281876991974</v>
+      </c>
+      <c r="D22">
+        <v>0.07529789264772963</v>
+      </c>
+      <c r="E22">
+        <v>0.4828810263023473</v>
+      </c>
+      <c r="F22">
+        <v>0.06949281876991974</v>
+      </c>
+      <c r="G22">
+        <v>1.401767971530121</v>
+      </c>
+      <c r="H22">
+        <v>0.07529789264772963</v>
+      </c>
+      <c r="I22">
+        <v>-0.0004574272900550851</v>
+      </c>
+      <c r="J22">
+        <v>0.01587949993991768</v>
+      </c>
+      <c r="K22">
+        <v>0.07529789264772963</v>
+      </c>
+      <c r="L22">
+        <v>0.4828810263023473</v>
+      </c>
+      <c r="M22">
+        <v>0.2761869225361335</v>
+      </c>
+      <c r="N22">
+        <v>0.2761869225361335</v>
+      </c>
+      <c r="O22">
+        <v>0.1839721392607373</v>
+      </c>
+      <c r="P22">
+        <v>0.2092239125733323</v>
+      </c>
+      <c r="Q22">
+        <v>0.2092239125733323</v>
+      </c>
+      <c r="R22">
+        <v>0.1757424075919316</v>
+      </c>
+      <c r="S22">
+        <v>0.1757424075919316</v>
+      </c>
+      <c r="T22">
+        <v>0.3408102969833302</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20">
+      <c r="A23" s="1">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23">
+        <v>0.0009906382284935978</v>
+      </c>
+      <c r="D23">
+        <v>1.650333686930785</v>
+      </c>
+      <c r="E23">
+        <v>0.9268749225926886</v>
+      </c>
+      <c r="F23">
+        <v>0.0009906382284935978</v>
+      </c>
+      <c r="G23">
+        <v>2.22350904549545</v>
+      </c>
+      <c r="H23">
+        <v>1.650333686930785</v>
+      </c>
+      <c r="I23">
+        <v>1.891613563536645</v>
+      </c>
+      <c r="J23">
+        <v>0.001147664018377604</v>
+      </c>
+      <c r="K23">
+        <v>1.650333686930785</v>
+      </c>
+      <c r="L23">
+        <v>0.9268749225926886</v>
+      </c>
+      <c r="M23">
+        <v>0.4639327804105911</v>
+      </c>
+      <c r="N23">
+        <v>0.4639327804105911</v>
+      </c>
+      <c r="O23">
+        <v>0.9398263747859422</v>
+      </c>
+      <c r="P23">
+        <v>0.8593997492506559</v>
+      </c>
+      <c r="Q23">
+        <v>0.8593997492506559</v>
+      </c>
+      <c r="R23">
+        <v>1.057133233670688</v>
+      </c>
+      <c r="S23">
+        <v>1.057133233670688</v>
+      </c>
+      <c r="T23">
+        <v>1.11574492013374</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20">
+      <c r="A24" s="1">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24">
+        <v>3.806806310651667</v>
+      </c>
+      <c r="D24">
+        <v>0.795381671876087</v>
+      </c>
+      <c r="E24">
+        <v>1.257223936975514</v>
+      </c>
+      <c r="F24">
+        <v>3.806806310651667</v>
+      </c>
+      <c r="G24">
+        <v>1.380876313850261</v>
+      </c>
+      <c r="H24">
+        <v>0.795381671876087</v>
+      </c>
+      <c r="I24">
+        <v>1.878161985072147</v>
+      </c>
+      <c r="J24">
+        <v>2.492586044649239</v>
+      </c>
+      <c r="K24">
+        <v>0.795381671876087</v>
+      </c>
+      <c r="L24">
+        <v>1.257223936975514</v>
+      </c>
+      <c r="M24">
+        <v>2.532015123813591</v>
+      </c>
+      <c r="N24">
+        <v>2.532015123813591</v>
+      </c>
+      <c r="O24">
+        <v>2.314064077566443</v>
+      </c>
+      <c r="P24">
+        <v>1.95313730650109</v>
+      </c>
+      <c r="Q24">
+        <v>1.953137306501089</v>
+      </c>
+      <c r="R24">
+        <v>1.663698397844839</v>
+      </c>
+      <c r="S24">
+        <v>1.663698397844839</v>
+      </c>
+      <c r="T24">
+        <v>1.935172710512486</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20">
+      <c r="A25" s="1">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>23</v>
+      </c>
+      <c r="C25">
+        <v>0.0005785544083198467</v>
+      </c>
+      <c r="D25">
+        <v>0.9221787154030172</v>
+      </c>
+      <c r="E25">
+        <v>3.207764372415052</v>
+      </c>
+      <c r="F25">
+        <v>0.0005785544083198467</v>
+      </c>
+      <c r="G25">
+        <v>0.01700950850845988</v>
+      </c>
+      <c r="H25">
+        <v>0.9221787154030172</v>
+      </c>
+      <c r="I25">
+        <v>0.006248484040885691</v>
+      </c>
+      <c r="J25">
+        <v>0.01141761173610538</v>
+      </c>
+      <c r="K25">
+        <v>0.9221787154030172</v>
+      </c>
+      <c r="L25">
+        <v>3.207764372415052</v>
+      </c>
+      <c r="M25">
+        <v>1.604171463411686</v>
+      </c>
+      <c r="N25">
+        <v>1.604171463411686</v>
+      </c>
+      <c r="O25">
+        <v>1.071530470288086</v>
+      </c>
+      <c r="P25">
+        <v>1.376840547408796</v>
+      </c>
+      <c r="Q25">
+        <v>1.376840547408796</v>
+      </c>
+      <c r="R25">
+        <v>1.263175089407352</v>
+      </c>
+      <c r="S25">
+        <v>1.263175089407352</v>
+      </c>
+      <c r="T25">
+        <v>0.6941995410853067</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20">
+      <c r="A26" s="1">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
+        <v>24</v>
+      </c>
+      <c r="C26">
+        <v>0.003145952570695001</v>
+      </c>
+      <c r="D26">
+        <v>0.009635403838611055</v>
+      </c>
+      <c r="E26">
+        <v>1.276966659993725</v>
+      </c>
+      <c r="F26">
+        <v>0.003145952570695001</v>
+      </c>
+      <c r="G26">
+        <v>1.00617965130892</v>
+      </c>
+      <c r="H26">
+        <v>0.009635403838611055</v>
+      </c>
+      <c r="I26">
+        <v>0.5721374030175033</v>
+      </c>
+      <c r="J26">
+        <v>1.859767807519045</v>
+      </c>
+      <c r="K26">
+        <v>0.009635403838611055</v>
+      </c>
+      <c r="L26">
+        <v>1.276966659993725</v>
+      </c>
+      <c r="M26">
+        <v>0.64005630628221</v>
+      </c>
+      <c r="N26">
+        <v>0.64005630628221</v>
+      </c>
+      <c r="O26">
+        <v>0.6174166718606411</v>
+      </c>
+      <c r="P26">
+        <v>0.429916005467677</v>
+      </c>
+      <c r="Q26">
+        <v>0.429916005467677</v>
+      </c>
+      <c r="R26">
+        <v>0.3248458550604105</v>
+      </c>
+      <c r="S26">
+        <v>0.3248458550604105</v>
+      </c>
+      <c r="T26">
+        <v>0.7879721463747499</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20">
+      <c r="A27" s="1">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>25</v>
+      </c>
+      <c r="C27">
+        <v>0.1226218843146754</v>
+      </c>
+      <c r="D27">
+        <v>1.145041287608157</v>
+      </c>
+      <c r="E27">
+        <v>0.0008891324879004232</v>
+      </c>
+      <c r="F27">
+        <v>0.1226218843146754</v>
+      </c>
+      <c r="G27">
+        <v>0.4632761339827141</v>
+      </c>
+      <c r="H27">
+        <v>1.145041287608157</v>
+      </c>
+      <c r="I27">
+        <v>0.006069047697103314</v>
+      </c>
+      <c r="J27">
+        <v>10.35736542542252</v>
+      </c>
+      <c r="K27">
+        <v>1.145041287608157</v>
+      </c>
+      <c r="L27">
+        <v>0.0008891324879004232</v>
+      </c>
+      <c r="M27">
+        <v>0.06175550840128793</v>
+      </c>
+      <c r="N27">
+        <v>0.06175550840128793</v>
+      </c>
+      <c r="O27">
+        <v>0.04319335483322639</v>
+      </c>
+      <c r="P27">
+        <v>0.4228507681369109</v>
+      </c>
+      <c r="Q27">
+        <v>0.4228507681369109</v>
+      </c>
+      <c r="R27">
+        <v>0.6033983980047224</v>
+      </c>
+      <c r="S27">
+        <v>0.6033983980047224</v>
+      </c>
+      <c r="T27">
+        <v>2.015877151918846</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20">
+      <c r="A28" s="1">
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
+        <v>26</v>
+      </c>
+      <c r="C28">
+        <v>0.03222520466330636</v>
+      </c>
+      <c r="D28">
+        <v>0.029784882913573</v>
+      </c>
+      <c r="E28">
+        <v>1.141624010106937</v>
+      </c>
+      <c r="F28">
+        <v>0.03222520466330636</v>
+      </c>
+      <c r="G28">
+        <v>1.822320010950573</v>
+      </c>
+      <c r="H28">
+        <v>0.029784882913573</v>
+      </c>
+      <c r="I28">
+        <v>1.404946126071093</v>
+      </c>
+      <c r="J28">
+        <v>0.003689391777067894</v>
+      </c>
+      <c r="K28">
+        <v>0.029784882913573</v>
+      </c>
+      <c r="L28">
+        <v>1.141624010106937</v>
+      </c>
+      <c r="M28">
+        <v>0.5869246073851218</v>
+      </c>
+      <c r="N28">
+        <v>0.5869246073851218</v>
+      </c>
+      <c r="O28">
+        <v>0.859598446947112</v>
+      </c>
+      <c r="P28">
+        <v>0.4012113658946055</v>
+      </c>
+      <c r="Q28">
+        <v>0.4012113658946055</v>
+      </c>
+      <c r="R28">
+        <v>0.3083547451493474</v>
+      </c>
+      <c r="S28">
+        <v>0.3083547451493474</v>
+      </c>
+      <c r="T28">
+        <v>0.739098271080425</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20">
+      <c r="A29" s="1">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>27</v>
+      </c>
+      <c r="C29">
+        <v>0.003650102051705286</v>
+      </c>
+      <c r="D29">
+        <v>-0.0007013616381167826</v>
+      </c>
+      <c r="E29">
+        <v>2.49730490468291</v>
+      </c>
+      <c r="F29">
+        <v>0.003650102051705286</v>
+      </c>
+      <c r="G29">
+        <v>0.7580881550873318</v>
+      </c>
+      <c r="H29">
+        <v>-0.0007013616381167826</v>
+      </c>
+      <c r="I29">
+        <v>2.893192146584329</v>
+      </c>
+      <c r="J29">
+        <v>-0.004807787644049314</v>
+      </c>
+      <c r="K29">
+        <v>-0.0007013616381167826</v>
+      </c>
+      <c r="L29">
+        <v>2.49730490468291</v>
+      </c>
+      <c r="M29">
+        <v>1.250477503367307</v>
+      </c>
+      <c r="N29">
+        <v>1.250477503367307</v>
+      </c>
+      <c r="O29">
+        <v>1.798049051106315</v>
+      </c>
+      <c r="P29">
+        <v>0.8334178816988328</v>
+      </c>
+      <c r="Q29">
+        <v>0.8334178816988328</v>
+      </c>
+      <c r="R29">
+        <v>0.6248880708645954</v>
+      </c>
+      <c r="S29">
+        <v>0.6248880708645954</v>
+      </c>
+      <c r="T29">
+        <v>1.024454359854018</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated notebook, reran simulation
</commit_message>
<xml_diff>
--- a/JupyterNotebooks/AvgHW/Alpha1F-HW03.xlsx
+++ b/JupyterNotebooks/AvgHW/Alpha1F-HW03.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>HKL</t>
   </si>
@@ -22,6 +22,12 @@
     <t>Spiral5</t>
   </si>
   <si>
+    <t>Holden</t>
+  </si>
+  <si>
+    <t>Rizzie Spiral</t>
+  </si>
+  <si>
     <t>RotRing OmegaMax-90</t>
   </si>
   <si>
@@ -37,7 +43,7 @@
     <t>Rizzie Hex</t>
   </si>
   <si>
-    <t>Thomas Hex</t>
+    <t>Matthies Hex</t>
   </si>
   <si>
     <t>Tilt Rotate_Partial</t>
@@ -509,7 +515,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T29"/>
+  <dimension ref="A1:T31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -582,58 +588,58 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="I2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="J2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="K2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="L2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="M2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="N2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="O2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="P2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="Q2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="R2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="S2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="T2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:20">
@@ -706,58 +712,58 @@
         <v>2</v>
       </c>
       <c r="C4">
-        <v>0.8845247616729527</v>
+        <v>1.254701697683301</v>
       </c>
       <c r="D4">
-        <v>1.082906649380325</v>
+        <v>0.7773705505138532</v>
       </c>
       <c r="E4">
-        <v>0.9551386270794382</v>
+        <v>0.8704374273154003</v>
       </c>
       <c r="F4">
-        <v>0.8845247616729527</v>
+        <v>1.254701697683301</v>
       </c>
       <c r="G4">
-        <v>1.047394633441321</v>
+        <v>0.8646450015213883</v>
       </c>
       <c r="H4">
-        <v>1.082906649380325</v>
+        <v>0.7773705505138532</v>
       </c>
       <c r="I4">
-        <v>0.7872592349169611</v>
+        <v>1.086051695758476</v>
       </c>
       <c r="J4">
-        <v>1.132495973221657</v>
+        <v>0.8237832698567501</v>
       </c>
       <c r="K4">
-        <v>1.082906649380325</v>
+        <v>0.7773705505138532</v>
       </c>
       <c r="L4">
-        <v>0.9551386270794382</v>
+        <v>0.8704374273154003</v>
       </c>
       <c r="M4">
-        <v>0.9198316943761955</v>
+        <v>1.062569562499351</v>
       </c>
       <c r="N4">
-        <v>0.9198316943761955</v>
+        <v>1.062569562499351</v>
       </c>
       <c r="O4">
-        <v>0.8756408745564507</v>
+        <v>1.070396940252393</v>
       </c>
       <c r="P4">
-        <v>0.9741900127109052</v>
+        <v>0.9675032251708516</v>
       </c>
       <c r="Q4">
-        <v>0.974190012710905</v>
+        <v>0.9675032251708516</v>
       </c>
       <c r="R4">
-        <v>1.00136917187826</v>
+        <v>0.919970056506602</v>
       </c>
       <c r="S4">
-        <v>1.00136917187826</v>
+        <v>0.919970056506602</v>
       </c>
       <c r="T4">
-        <v>0.981619979952109</v>
+        <v>0.9461649404415283</v>
       </c>
     </row>
     <row r="5" spans="1:20">
@@ -768,58 +774,58 @@
         <v>3</v>
       </c>
       <c r="C5">
-        <v>1.173761791692285</v>
+        <v>0.001351506250955896</v>
       </c>
       <c r="D5">
-        <v>0.9988664757047482</v>
+        <v>4.492740714395812</v>
       </c>
       <c r="E5">
-        <v>0.8143293733694247</v>
+        <v>0.001944713813196694</v>
       </c>
       <c r="F5">
-        <v>1.173761791692285</v>
+        <v>0.001351506250955896</v>
       </c>
       <c r="G5">
-        <v>0.8630531185074014</v>
+        <v>1.241745914772147</v>
       </c>
       <c r="H5">
-        <v>0.9988664757047482</v>
+        <v>4.492740714395812</v>
       </c>
       <c r="I5">
-        <v>1.040072132954511</v>
+        <v>1.802594376952982</v>
       </c>
       <c r="J5">
-        <v>0.7708217850544109</v>
+        <v>0.01102323034015119</v>
       </c>
       <c r="K5">
-        <v>0.9988664757047482</v>
+        <v>4.492740714395812</v>
       </c>
       <c r="L5">
-        <v>0.8143293733694247</v>
+        <v>0.001944713813196694</v>
       </c>
       <c r="M5">
-        <v>0.9940455825308547</v>
+        <v>0.001648110032076296</v>
       </c>
       <c r="N5">
-        <v>0.9940455825308547</v>
+        <v>0.001648110032076296</v>
       </c>
       <c r="O5">
-        <v>1.009387766005407</v>
+        <v>0.6019635323390449</v>
       </c>
       <c r="P5">
-        <v>0.9956525469221525</v>
+        <v>1.498678978153322</v>
       </c>
       <c r="Q5">
-        <v>0.9956525469221525</v>
+        <v>1.498678978153322</v>
       </c>
       <c r="R5">
-        <v>0.9964560291178014</v>
+        <v>2.247194412213944</v>
       </c>
       <c r="S5">
-        <v>0.9964560291178014</v>
+        <v>2.247194412213944</v>
       </c>
       <c r="T5">
-        <v>0.9434841128804634</v>
+        <v>1.258566742754207</v>
       </c>
     </row>
     <row r="6" spans="1:20">
@@ -830,58 +836,58 @@
         <v>4</v>
       </c>
       <c r="C6">
-        <v>0.5787035104381049</v>
+        <v>0.8845247616729527</v>
       </c>
       <c r="D6">
-        <v>0.4662126205697955</v>
+        <v>1.082906649380325</v>
       </c>
       <c r="E6">
-        <v>0.4591235400880798</v>
+        <v>0.9551386270794382</v>
       </c>
       <c r="F6">
-        <v>0.5787035104381049</v>
+        <v>0.8845247616729527</v>
       </c>
       <c r="G6">
-        <v>0.436242668215461</v>
+        <v>1.047394633441321</v>
       </c>
       <c r="H6">
-        <v>0.4662126205697955</v>
+        <v>1.082906649380325</v>
       </c>
       <c r="I6">
-        <v>0.5441068785151475</v>
+        <v>0.7872592349169611</v>
       </c>
       <c r="J6">
-        <v>0.4232749538598622</v>
+        <v>1.132495973221657</v>
       </c>
       <c r="K6">
-        <v>0.4662126205697955</v>
+        <v>1.082906649380325</v>
       </c>
       <c r="L6">
-        <v>0.4591235400880798</v>
+        <v>0.9551386270794382</v>
       </c>
       <c r="M6">
-        <v>0.5189135252630923</v>
+        <v>0.9198316943761955</v>
       </c>
       <c r="N6">
-        <v>0.5189135252630923</v>
+        <v>0.9198316943761955</v>
       </c>
       <c r="O6">
-        <v>0.527311309680444</v>
+        <v>0.8756408745564507</v>
       </c>
       <c r="P6">
-        <v>0.5013465570319934</v>
+        <v>0.9741900127109052</v>
       </c>
       <c r="Q6">
-        <v>0.5013465570319934</v>
+        <v>0.974190012710905</v>
       </c>
       <c r="R6">
-        <v>0.4925630729164439</v>
+        <v>1.00136917187826</v>
       </c>
       <c r="S6">
-        <v>0.4925630729164439</v>
+        <v>1.00136917187826</v>
       </c>
       <c r="T6">
-        <v>0.4846106952810751</v>
+        <v>0.981619979952109</v>
       </c>
     </row>
     <row r="7" spans="1:20">
@@ -892,58 +898,58 @@
         <v>5</v>
       </c>
       <c r="C7">
-        <v>0.9846422066275502</v>
+        <v>1.173761791692285</v>
       </c>
       <c r="D7">
-        <v>1.146734370382373</v>
+        <v>0.9988664757047482</v>
       </c>
       <c r="E7">
-        <v>0.9237831735460421</v>
+        <v>0.8143293733694247</v>
       </c>
       <c r="F7">
-        <v>0.9846422066275502</v>
+        <v>1.173761791692285</v>
       </c>
       <c r="G7">
-        <v>1.054145349892974</v>
+        <v>0.8630531185074014</v>
       </c>
       <c r="H7">
-        <v>1.146734370382373</v>
+        <v>0.9988664757047482</v>
       </c>
       <c r="I7">
-        <v>0.9458238522669338</v>
+        <v>1.040072132954511</v>
       </c>
       <c r="J7">
-        <v>0.9646010997971536</v>
+        <v>0.7708217850544109</v>
       </c>
       <c r="K7">
-        <v>1.146734370382373</v>
+        <v>0.9988664757047482</v>
       </c>
       <c r="L7">
-        <v>0.9237831735460421</v>
+        <v>0.8143293733694247</v>
       </c>
       <c r="M7">
-        <v>0.9542126900867962</v>
+        <v>0.9940455825308547</v>
       </c>
       <c r="N7">
-        <v>0.9542126900867962</v>
+        <v>0.9940455825308547</v>
       </c>
       <c r="O7">
-        <v>0.9514164108135087</v>
+        <v>1.009387766005407</v>
       </c>
       <c r="P7">
-        <v>1.018386583518655</v>
+        <v>0.9956525469221525</v>
       </c>
       <c r="Q7">
-        <v>1.018386583518655</v>
+        <v>0.9956525469221525</v>
       </c>
       <c r="R7">
-        <v>1.050473530234584</v>
+        <v>0.9964560291178014</v>
       </c>
       <c r="S7">
-        <v>1.050473530234584</v>
+        <v>0.9964560291178014</v>
       </c>
       <c r="T7">
-        <v>1.003288342085504</v>
+        <v>0.9434841128804634</v>
       </c>
     </row>
     <row r="8" spans="1:20">
@@ -954,58 +960,58 @@
         <v>6</v>
       </c>
       <c r="C8">
-        <v>0.9722130771406368</v>
+        <v>0.5787035104381049</v>
       </c>
       <c r="D8">
-        <v>1.142308003872336</v>
+        <v>0.4662126205697955</v>
       </c>
       <c r="E8">
-        <v>0.9856795263322912</v>
+        <v>0.4591235400880798</v>
       </c>
       <c r="F8">
-        <v>0.9722130771406368</v>
+        <v>0.5787035104381049</v>
       </c>
       <c r="G8">
-        <v>1.007890703643511</v>
+        <v>0.436242668215461</v>
       </c>
       <c r="H8">
-        <v>1.142308003872336</v>
+        <v>0.4662126205697955</v>
       </c>
       <c r="I8">
-        <v>0.9623569163748993</v>
+        <v>0.5441068785151475</v>
       </c>
       <c r="J8">
-        <v>1.02187662150615</v>
+        <v>0.4232749538598622</v>
       </c>
       <c r="K8">
-        <v>1.142308003872336</v>
+        <v>0.4662126205697955</v>
       </c>
       <c r="L8">
-        <v>0.9856795263322912</v>
+        <v>0.4591235400880798</v>
       </c>
       <c r="M8">
-        <v>0.9789463017364639</v>
+        <v>0.5189135252630923</v>
       </c>
       <c r="N8">
-        <v>0.9789463017364639</v>
+        <v>0.5189135252630923</v>
       </c>
       <c r="O8">
-        <v>0.9734165066159424</v>
+        <v>0.527311309680444</v>
       </c>
       <c r="P8">
-        <v>1.033400202448421</v>
+        <v>0.5013465570319934</v>
       </c>
       <c r="Q8">
-        <v>1.033400202448421</v>
+        <v>0.5013465570319934</v>
       </c>
       <c r="R8">
-        <v>1.0606271528044</v>
+        <v>0.4925630729164439</v>
       </c>
       <c r="S8">
-        <v>1.0606271528044</v>
+        <v>0.4925630729164439</v>
       </c>
       <c r="T8">
-        <v>1.015387474811637</v>
+        <v>0.4846106952810751</v>
       </c>
     </row>
     <row r="9" spans="1:20">
@@ -1016,58 +1022,58 @@
         <v>7</v>
       </c>
       <c r="C9">
-        <v>1.225419474706893</v>
+        <v>0.9846422066275502</v>
       </c>
       <c r="D9">
-        <v>1.291315184167343</v>
+        <v>1.146734370382373</v>
       </c>
       <c r="E9">
-        <v>0.9281919766583274</v>
+        <v>0.9237831735460421</v>
       </c>
       <c r="F9">
-        <v>1.225419474706893</v>
+        <v>0.9846422066275502</v>
       </c>
       <c r="G9">
-        <v>1.143606536477421</v>
+        <v>1.054145349892974</v>
       </c>
       <c r="H9">
-        <v>1.291315184167343</v>
+        <v>1.146734370382373</v>
       </c>
       <c r="I9">
-        <v>0.7039957044935053</v>
+        <v>0.9458238522669338</v>
       </c>
       <c r="J9">
-        <v>1.008385953488546</v>
+        <v>0.9646010997971536</v>
       </c>
       <c r="K9">
-        <v>1.291315184167343</v>
+        <v>1.146734370382373</v>
       </c>
       <c r="L9">
-        <v>0.9281919766583274</v>
+        <v>0.9237831735460421</v>
       </c>
       <c r="M9">
-        <v>1.07680572568261</v>
+        <v>0.9542126900867962</v>
       </c>
       <c r="N9">
-        <v>1.07680572568261</v>
+        <v>0.9542126900867962</v>
       </c>
       <c r="O9">
-        <v>0.9525357186195751</v>
+        <v>0.9514164108135087</v>
       </c>
       <c r="P9">
-        <v>1.148308878510854</v>
+        <v>1.018386583518655</v>
       </c>
       <c r="Q9">
-        <v>1.148308878510854</v>
+        <v>1.018386583518655</v>
       </c>
       <c r="R9">
-        <v>1.184060454924976</v>
+        <v>1.050473530234584</v>
       </c>
       <c r="S9">
-        <v>1.184060454924976</v>
+        <v>1.050473530234584</v>
       </c>
       <c r="T9">
-        <v>1.050152471665339</v>
+        <v>1.003288342085504</v>
       </c>
     </row>
     <row r="10" spans="1:20">
@@ -1078,58 +1084,58 @@
         <v>8</v>
       </c>
       <c r="C10">
-        <v>0.6069740241260413</v>
+        <v>0.9722130771406368</v>
       </c>
       <c r="D10">
-        <v>0.4421357857954734</v>
+        <v>1.142308003872336</v>
       </c>
       <c r="E10">
-        <v>0.4273157588461299</v>
+        <v>0.9856795263322912</v>
       </c>
       <c r="F10">
-        <v>0.6069740241260413</v>
+        <v>0.9722130771406368</v>
       </c>
       <c r="G10">
-        <v>0.4167866881363111</v>
+        <v>1.007890703643511</v>
       </c>
       <c r="H10">
-        <v>0.4421357857954734</v>
+        <v>1.142308003872336</v>
       </c>
       <c r="I10">
-        <v>0.5485888796317363</v>
+        <v>0.9623569163748993</v>
       </c>
       <c r="J10">
-        <v>0.4595612543949866</v>
+        <v>1.02187662150615</v>
       </c>
       <c r="K10">
-        <v>0.4421357857954734</v>
+        <v>1.142308003872336</v>
       </c>
       <c r="L10">
-        <v>0.4273157588461299</v>
+        <v>0.9856795263322912</v>
       </c>
       <c r="M10">
-        <v>0.5171448914860856</v>
+        <v>0.9789463017364639</v>
       </c>
       <c r="N10">
-        <v>0.5171448914860856</v>
+        <v>0.9789463017364639</v>
       </c>
       <c r="O10">
-        <v>0.5276262208679691</v>
+        <v>0.9734165066159424</v>
       </c>
       <c r="P10">
-        <v>0.4921418562558815</v>
+        <v>1.033400202448421</v>
       </c>
       <c r="Q10">
-        <v>0.4921418562558815</v>
+        <v>1.033400202448421</v>
       </c>
       <c r="R10">
-        <v>0.4796403386407794</v>
+        <v>1.0606271528044</v>
       </c>
       <c r="S10">
-        <v>0.4796403386407794</v>
+        <v>1.0606271528044</v>
       </c>
       <c r="T10">
-        <v>0.4835603984884465</v>
+        <v>1.015387474811637</v>
       </c>
     </row>
     <row r="11" spans="1:20">
@@ -1140,58 +1146,58 @@
         <v>9</v>
       </c>
       <c r="C11">
-        <v>0.8723211855978082</v>
+        <v>1.225419474706893</v>
       </c>
       <c r="D11">
-        <v>0.8611351388353655</v>
+        <v>1.291315184167343</v>
       </c>
       <c r="E11">
-        <v>0.9851915386376003</v>
+        <v>0.9281919766583274</v>
       </c>
       <c r="F11">
-        <v>0.8723211855978082</v>
+        <v>1.225419474706893</v>
       </c>
       <c r="G11">
-        <v>1.19771356375457</v>
+        <v>1.143606536477421</v>
       </c>
       <c r="H11">
-        <v>0.8611351388353655</v>
+        <v>1.291315184167343</v>
       </c>
       <c r="I11">
-        <v>0.8543971311857294</v>
+        <v>0.7039957044935053</v>
       </c>
       <c r="J11">
-        <v>0.4570903765846644</v>
+        <v>1.008385953488546</v>
       </c>
       <c r="K11">
-        <v>0.8611351388353655</v>
+        <v>1.291315184167343</v>
       </c>
       <c r="L11">
-        <v>0.9851915386376003</v>
+        <v>0.9281919766583274</v>
       </c>
       <c r="M11">
-        <v>0.9287563621177043</v>
+        <v>1.07680572568261</v>
       </c>
       <c r="N11">
-        <v>0.9287563621177043</v>
+        <v>1.07680572568261</v>
       </c>
       <c r="O11">
-        <v>0.903969951807046</v>
+        <v>0.9525357186195751</v>
       </c>
       <c r="P11">
-        <v>0.9062159543569247</v>
+        <v>1.148308878510854</v>
       </c>
       <c r="Q11">
-        <v>0.9062159543569247</v>
+        <v>1.148308878510854</v>
       </c>
       <c r="R11">
-        <v>0.8949457504765349</v>
+        <v>1.184060454924976</v>
       </c>
       <c r="S11">
-        <v>0.8949457504765349</v>
+        <v>1.184060454924976</v>
       </c>
       <c r="T11">
-        <v>0.8713081557659564</v>
+        <v>1.050152471665339</v>
       </c>
     </row>
     <row r="12" spans="1:20">
@@ -1202,58 +1208,58 @@
         <v>10</v>
       </c>
       <c r="C12">
-        <v>1.11308471458956</v>
+        <v>0.6069740241260413</v>
       </c>
       <c r="D12">
-        <v>0.8571234646570741</v>
+        <v>0.4421357857954734</v>
       </c>
       <c r="E12">
-        <v>0.8428092352636376</v>
+        <v>0.4273157588461299</v>
       </c>
       <c r="F12">
-        <v>1.11308471458956</v>
+        <v>0.6069740241260413</v>
       </c>
       <c r="G12">
-        <v>0.8127840244326886</v>
+        <v>0.4167866881363111</v>
       </c>
       <c r="H12">
-        <v>0.8571234646570741</v>
+        <v>0.4421357857954734</v>
       </c>
       <c r="I12">
-        <v>1.073065520892483</v>
+        <v>0.5485888796317363</v>
       </c>
       <c r="J12">
-        <v>0.876702440456508</v>
+        <v>0.4595612543949866</v>
       </c>
       <c r="K12">
-        <v>0.8571234646570741</v>
+        <v>0.4421357857954734</v>
       </c>
       <c r="L12">
-        <v>0.8428092352636376</v>
+        <v>0.4273157588461299</v>
       </c>
       <c r="M12">
-        <v>0.9779469749265987</v>
+        <v>0.5171448914860856</v>
       </c>
       <c r="N12">
-        <v>0.9779469749265987</v>
+        <v>0.5171448914860856</v>
       </c>
       <c r="O12">
-        <v>1.009653156915227</v>
+        <v>0.5276262208679691</v>
       </c>
       <c r="P12">
-        <v>0.9376724715034238</v>
+        <v>0.4921418562558815</v>
       </c>
       <c r="Q12">
-        <v>0.9376724715034239</v>
+        <v>0.4921418562558815</v>
       </c>
       <c r="R12">
-        <v>0.9175352197918365</v>
+        <v>0.4796403386407794</v>
       </c>
       <c r="S12">
-        <v>0.9175352197918365</v>
+        <v>0.4796403386407794</v>
       </c>
       <c r="T12">
-        <v>0.9292615667153252</v>
+        <v>0.4835603984884465</v>
       </c>
     </row>
     <row r="13" spans="1:20">
@@ -1264,58 +1270,58 @@
         <v>11</v>
       </c>
       <c r="C13">
-        <v>0.6699817763633297</v>
+        <v>0.8723211855978082</v>
       </c>
       <c r="D13">
-        <v>1.271008044503521</v>
+        <v>0.8611351388353655</v>
       </c>
       <c r="E13">
-        <v>1.115278358379869</v>
+        <v>0.9851915386376003</v>
       </c>
       <c r="F13">
-        <v>0.6699817763633297</v>
+        <v>0.8723211855978082</v>
       </c>
       <c r="G13">
-        <v>1.087123251781193</v>
+        <v>1.19771356375457</v>
       </c>
       <c r="H13">
-        <v>1.271008044503521</v>
+        <v>0.8611351388353655</v>
       </c>
       <c r="I13">
-        <v>0.7746128494181943</v>
+        <v>0.8543971311857294</v>
       </c>
       <c r="J13">
-        <v>1.410886158389823</v>
+        <v>0.4570903765846644</v>
       </c>
       <c r="K13">
-        <v>1.271008044503521</v>
+        <v>0.8611351388353655</v>
       </c>
       <c r="L13">
-        <v>1.115278358379869</v>
+        <v>0.9851915386376003</v>
       </c>
       <c r="M13">
-        <v>0.8926300673715994</v>
+        <v>0.9287563621177043</v>
       </c>
       <c r="N13">
-        <v>0.8926300673715994</v>
+        <v>0.9287563621177043</v>
       </c>
       <c r="O13">
-        <v>0.8532909947204644</v>
+        <v>0.903969951807046</v>
       </c>
       <c r="P13">
-        <v>1.018756059748907</v>
+        <v>0.9062159543569247</v>
       </c>
       <c r="Q13">
-        <v>1.018756059748907</v>
+        <v>0.9062159543569247</v>
       </c>
       <c r="R13">
-        <v>1.08181905593756</v>
+        <v>0.8949457504765349</v>
       </c>
       <c r="S13">
-        <v>1.08181905593756</v>
+        <v>0.8949457504765349</v>
       </c>
       <c r="T13">
-        <v>1.054815073139322</v>
+        <v>0.8713081557659564</v>
       </c>
     </row>
     <row r="14" spans="1:20">
@@ -1326,58 +1332,58 @@
         <v>12</v>
       </c>
       <c r="C14">
-        <v>-0.01248147300000001</v>
+        <v>1.11308471458956</v>
       </c>
       <c r="D14">
-        <v>-0.0009139994799999984</v>
+        <v>0.8571234646570741</v>
       </c>
       <c r="E14">
-        <v>-0.010207482</v>
+        <v>0.8428092352636376</v>
       </c>
       <c r="F14">
-        <v>-0.01248147300000001</v>
+        <v>1.11308471458956</v>
       </c>
       <c r="G14">
-        <v>0.005017741899999998</v>
+        <v>0.8127840244326886</v>
       </c>
       <c r="H14">
-        <v>-0.0009139994799999984</v>
+        <v>0.8571234646570741</v>
       </c>
       <c r="I14">
-        <v>0.024963772</v>
+        <v>1.073065520892483</v>
       </c>
       <c r="J14">
-        <v>0.004912388499999995</v>
+        <v>0.876702440456508</v>
       </c>
       <c r="K14">
-        <v>-0.0009139994799999984</v>
+        <v>0.8571234646570741</v>
       </c>
       <c r="L14">
-        <v>-0.010207482</v>
+        <v>0.8428092352636376</v>
       </c>
       <c r="M14">
-        <v>-0.01134447750000001</v>
+        <v>0.9779469749265987</v>
       </c>
       <c r="N14">
-        <v>-0.01134447750000001</v>
+        <v>0.9779469749265987</v>
       </c>
       <c r="O14">
-        <v>0.0007582723333333293</v>
+        <v>1.009653156915227</v>
       </c>
       <c r="P14">
-        <v>-0.007867651493333336</v>
+        <v>0.9376724715034238</v>
       </c>
       <c r="Q14">
-        <v>-0.007867651493333336</v>
+        <v>0.9376724715034239</v>
       </c>
       <c r="R14">
-        <v>-0.006129238490000001</v>
+        <v>0.9175352197918365</v>
       </c>
       <c r="S14">
-        <v>-0.006129238490000001</v>
+        <v>0.9175352197918365</v>
       </c>
       <c r="T14">
-        <v>0.001881824653333331</v>
+        <v>0.9292615667153252</v>
       </c>
     </row>
     <row r="15" spans="1:20">
@@ -1388,58 +1394,58 @@
         <v>13</v>
       </c>
       <c r="C15">
-        <v>0.00070900843</v>
+        <v>0.6699817763633297</v>
       </c>
       <c r="D15">
-        <v>121.14151</v>
+        <v>1.271008044503521</v>
       </c>
       <c r="E15">
-        <v>-0.012240956</v>
+        <v>1.115278358379869</v>
       </c>
       <c r="F15">
-        <v>0.00070900843</v>
+        <v>0.6699817763633297</v>
       </c>
       <c r="G15">
-        <v>-0.0067091534</v>
+        <v>1.087123251781193</v>
       </c>
       <c r="H15">
-        <v>121.14151</v>
+        <v>1.271008044503521</v>
       </c>
       <c r="I15">
-        <v>-0.0017802751</v>
+        <v>0.7746128494181943</v>
       </c>
       <c r="J15">
-        <v>0.010282672</v>
+        <v>1.410886158389823</v>
       </c>
       <c r="K15">
-        <v>121.14151</v>
+        <v>1.271008044503521</v>
       </c>
       <c r="L15">
-        <v>-0.012240956</v>
+        <v>1.115278358379869</v>
       </c>
       <c r="M15">
-        <v>-0.005765973785000001</v>
+        <v>0.8926300673715994</v>
       </c>
       <c r="N15">
-        <v>-0.005765973785000001</v>
+        <v>0.8926300673715994</v>
       </c>
       <c r="O15">
-        <v>-0.004437407556666668</v>
+        <v>0.8532909947204644</v>
       </c>
       <c r="P15">
-        <v>40.37665935080999</v>
+        <v>1.018756059748907</v>
       </c>
       <c r="Q15">
-        <v>40.37665935080999</v>
+        <v>1.018756059748907</v>
       </c>
       <c r="R15">
-        <v>60.5678720131075</v>
+        <v>1.08181905593756</v>
       </c>
       <c r="S15">
-        <v>60.5678720131075</v>
+        <v>1.08181905593756</v>
       </c>
       <c r="T15">
-        <v>20.18862854932167</v>
+        <v>1.054815073139322</v>
       </c>
     </row>
     <row r="16" spans="1:20">
@@ -1450,58 +1456,58 @@
         <v>14</v>
       </c>
       <c r="C16">
-        <v>0.016549232</v>
+        <v>-0.01248147300000001</v>
       </c>
       <c r="D16">
-        <v>-0.0025525058</v>
+        <v>-0.0009139994799999984</v>
       </c>
       <c r="E16">
-        <v>-0.010349456</v>
+        <v>-0.010207482</v>
       </c>
       <c r="F16">
-        <v>0.016549232</v>
+        <v>-0.01248147300000001</v>
       </c>
       <c r="G16">
-        <v>-0.0019770734</v>
+        <v>0.005017741899999998</v>
       </c>
       <c r="H16">
-        <v>-0.0025525058</v>
+        <v>-0.0009139994799999984</v>
       </c>
       <c r="I16">
-        <v>-0.011953383</v>
+        <v>0.024963772</v>
       </c>
       <c r="J16">
-        <v>-0.017342988</v>
+        <v>0.004912388499999995</v>
       </c>
       <c r="K16">
-        <v>-0.0025525058</v>
+        <v>-0.0009139994799999984</v>
       </c>
       <c r="L16">
-        <v>-0.010349456</v>
+        <v>-0.010207482</v>
       </c>
       <c r="M16">
-        <v>0.003099888</v>
+        <v>-0.01134447750000001</v>
       </c>
       <c r="N16">
-        <v>0.003099888</v>
+        <v>-0.01134447750000001</v>
       </c>
       <c r="O16">
-        <v>-0.001917869</v>
+        <v>0.0007582723333333293</v>
       </c>
       <c r="P16">
-        <v>0.001215756733333334</v>
+        <v>-0.007867651493333336</v>
       </c>
       <c r="Q16">
-        <v>0.001215756733333333</v>
+        <v>-0.007867651493333336</v>
       </c>
       <c r="R16">
-        <v>0.0002736911000000001</v>
+        <v>-0.006129238490000001</v>
       </c>
       <c r="S16">
-        <v>0.0002736911000000001</v>
+        <v>-0.006129238490000001</v>
       </c>
       <c r="T16">
-        <v>-0.004604362366666667</v>
+        <v>0.001881824653333331</v>
       </c>
     </row>
     <row r="17" spans="1:20">
@@ -1512,58 +1518,58 @@
         <v>15</v>
       </c>
       <c r="C17">
-        <v>-0.00014894864</v>
+        <v>0.00070900843</v>
       </c>
       <c r="D17">
-        <v>-0.0057702847</v>
+        <v>121.14151</v>
       </c>
       <c r="E17">
-        <v>0.0021540222</v>
+        <v>-0.012240956</v>
       </c>
       <c r="F17">
-        <v>-0.00014894864</v>
+        <v>0.00070900843</v>
       </c>
       <c r="G17">
-        <v>-0.0039257384</v>
+        <v>-0.0067091534</v>
       </c>
       <c r="H17">
-        <v>-0.0057702847</v>
+        <v>121.14151</v>
       </c>
       <c r="I17">
-        <v>0.00088323181</v>
+        <v>-0.0017802751</v>
       </c>
       <c r="J17">
-        <v>0.0043434522</v>
+        <v>0.010282672</v>
       </c>
       <c r="K17">
-        <v>-0.0057702847</v>
+        <v>121.14151</v>
       </c>
       <c r="L17">
-        <v>0.0021540222</v>
+        <v>-0.012240956</v>
       </c>
       <c r="M17">
-        <v>0.00100253678</v>
+        <v>-0.005765973785000001</v>
       </c>
       <c r="N17">
-        <v>0.00100253678</v>
+        <v>-0.005765973785000001</v>
       </c>
       <c r="O17">
-        <v>0.0009627684566666667</v>
+        <v>-0.004437407556666668</v>
       </c>
       <c r="P17">
-        <v>-0.00125507038</v>
+        <v>40.37665935080999</v>
       </c>
       <c r="Q17">
-        <v>-0.00125507038</v>
+        <v>40.37665935080999</v>
       </c>
       <c r="R17">
-        <v>-0.00238387396</v>
+        <v>60.5678720131075</v>
       </c>
       <c r="S17">
-        <v>-0.00238387396</v>
+        <v>60.5678720131075</v>
       </c>
       <c r="T17">
-        <v>-0.0004107109216666668</v>
+        <v>20.18862854932167</v>
       </c>
     </row>
     <row r="18" spans="1:20">
@@ -1574,58 +1580,58 @@
         <v>16</v>
       </c>
       <c r="C18">
-        <v>-0.005294425011917811</v>
+        <v>0.016549232</v>
       </c>
       <c r="D18">
-        <v>5.395919898593863</v>
+        <v>-0.0025525058</v>
       </c>
       <c r="E18">
-        <v>0.0006851950339726029</v>
+        <v>-0.010349456</v>
       </c>
       <c r="F18">
-        <v>-0.005294425011917811</v>
+        <v>0.016549232</v>
       </c>
       <c r="G18">
-        <v>1.811715642742466</v>
+        <v>-0.0019770734</v>
       </c>
       <c r="H18">
-        <v>5.395919898593863</v>
+        <v>-0.0025525058</v>
       </c>
       <c r="I18">
-        <v>0.02582977893013699</v>
+        <v>-0.011953383</v>
       </c>
       <c r="J18">
-        <v>0.0003422312493150687</v>
+        <v>-0.017342988</v>
       </c>
       <c r="K18">
-        <v>5.395919898593863</v>
+        <v>-0.0025525058</v>
       </c>
       <c r="L18">
-        <v>0.0006851950339726029</v>
+        <v>-0.010349456</v>
       </c>
       <c r="M18">
-        <v>-0.002304614988972604</v>
+        <v>0.003099888</v>
       </c>
       <c r="N18">
-        <v>-0.002304614988972604</v>
+        <v>0.003099888</v>
       </c>
       <c r="O18">
-        <v>0.00707351631739726</v>
+        <v>-0.001917869</v>
       </c>
       <c r="P18">
-        <v>1.797103556205306</v>
+        <v>0.001215756733333334</v>
       </c>
       <c r="Q18">
-        <v>1.797103556205306</v>
+        <v>0.001215756733333333</v>
       </c>
       <c r="R18">
-        <v>2.696807641802445</v>
+        <v>0.0002736911000000001</v>
       </c>
       <c r="S18">
-        <v>2.696807641802445</v>
+        <v>0.0002736911000000001</v>
       </c>
       <c r="T18">
-        <v>1.204866386922973</v>
+        <v>-0.004604362366666667</v>
       </c>
     </row>
     <row r="19" spans="1:20">
@@ -1636,58 +1642,58 @@
         <v>17</v>
       </c>
       <c r="C19">
-        <v>7.002471562811579</v>
+        <v>-0.00014894864</v>
       </c>
       <c r="D19">
-        <v>3.501838080206315</v>
+        <v>-0.0057702847</v>
       </c>
       <c r="E19">
-        <v>3.496064890227895</v>
+        <v>0.0021540222</v>
       </c>
       <c r="F19">
-        <v>7.002471562811579</v>
+        <v>-0.00014894864</v>
       </c>
       <c r="G19">
-        <v>-0.005191953220894737</v>
+        <v>-0.0039257384</v>
       </c>
       <c r="H19">
-        <v>3.501838080206315</v>
+        <v>-0.0057702847</v>
       </c>
       <c r="I19">
-        <v>0.001817788109157895</v>
+        <v>0.00088323181</v>
       </c>
       <c r="J19">
-        <v>10.48957806246842</v>
+        <v>0.0043434522</v>
       </c>
       <c r="K19">
-        <v>3.501838080206315</v>
+        <v>-0.0057702847</v>
       </c>
       <c r="L19">
-        <v>3.496064890227895</v>
+        <v>0.0021540222</v>
       </c>
       <c r="M19">
-        <v>5.249268226519737</v>
+        <v>0.00100253678</v>
       </c>
       <c r="N19">
-        <v>5.249268226519737</v>
+        <v>0.00100253678</v>
       </c>
       <c r="O19">
-        <v>3.500118080382877</v>
+        <v>0.0009627684566666667</v>
       </c>
       <c r="P19">
-        <v>4.66679151108193</v>
+        <v>-0.00125507038</v>
       </c>
       <c r="Q19">
-        <v>4.66679151108193</v>
+        <v>-0.00125507038</v>
       </c>
       <c r="R19">
-        <v>4.375553153363026</v>
+        <v>-0.00238387396</v>
       </c>
       <c r="S19">
-        <v>4.375553153363026</v>
+        <v>-0.00238387396</v>
       </c>
       <c r="T19">
-        <v>4.081096405100413</v>
+        <v>-0.0004107109216666668</v>
       </c>
     </row>
     <row r="20" spans="1:20">
@@ -1698,58 +1704,58 @@
         <v>18</v>
       </c>
       <c r="C20">
-        <v>0.001358614239473684</v>
+        <v>-0.005294425011917811</v>
       </c>
       <c r="D20">
-        <v>6.778065580148422</v>
+        <v>5.395919898593863</v>
       </c>
       <c r="E20">
-        <v>0.0009891908884210525</v>
+        <v>0.0006851950339726029</v>
       </c>
       <c r="F20">
-        <v>0.001358614239473684</v>
+        <v>-0.005294425011917811</v>
       </c>
       <c r="G20">
-        <v>1.124473584028421</v>
+        <v>1.811715642742466</v>
       </c>
       <c r="H20">
-        <v>6.778065580148422</v>
+        <v>5.395919898593863</v>
       </c>
       <c r="I20">
-        <v>1.647539540644316</v>
+        <v>0.02582977893013699</v>
       </c>
       <c r="J20">
-        <v>0.01061339926157895</v>
+        <v>0.0003422312493150687</v>
       </c>
       <c r="K20">
-        <v>6.778065580148422</v>
+        <v>5.395919898593863</v>
       </c>
       <c r="L20">
-        <v>0.0009891908884210525</v>
+        <v>0.0006851950339726029</v>
       </c>
       <c r="M20">
-        <v>0.001173902563947368</v>
+        <v>-0.002304614988972604</v>
       </c>
       <c r="N20">
-        <v>0.001173902563947368</v>
+        <v>-0.002304614988972604</v>
       </c>
       <c r="O20">
-        <v>0.5499624485907368</v>
+        <v>0.00707351631739726</v>
       </c>
       <c r="P20">
-        <v>2.260137795092105</v>
+        <v>1.797103556205306</v>
       </c>
       <c r="Q20">
-        <v>2.260137795092105</v>
+        <v>1.797103556205306</v>
       </c>
       <c r="R20">
-        <v>3.389619741356184</v>
+        <v>2.696807641802445</v>
       </c>
       <c r="S20">
-        <v>3.389619741356184</v>
+        <v>2.696807641802445</v>
       </c>
       <c r="T20">
-        <v>1.593839984868439</v>
+        <v>1.204866386922973</v>
       </c>
     </row>
     <row r="21" spans="1:20">
@@ -1760,58 +1766,58 @@
         <v>19</v>
       </c>
       <c r="C21">
-        <v>0.5490285290253076</v>
+        <v>7.002471562811579</v>
       </c>
       <c r="D21">
-        <v>-0.000758429579418342</v>
+        <v>3.501838080206315</v>
       </c>
       <c r="E21">
-        <v>1.694874496173247</v>
+        <v>3.496064890227895</v>
       </c>
       <c r="F21">
-        <v>0.5490285290253076</v>
+        <v>7.002471562811579</v>
       </c>
       <c r="G21">
-        <v>0.09679846039972893</v>
+        <v>-0.005191953220894737</v>
       </c>
       <c r="H21">
-        <v>-0.000758429579418342</v>
+        <v>3.501838080206315</v>
       </c>
       <c r="I21">
-        <v>2.163906465814728</v>
+        <v>0.001817788109157895</v>
       </c>
       <c r="J21">
-        <v>0.07992494560801601</v>
+        <v>10.48957806246842</v>
       </c>
       <c r="K21">
-        <v>-0.000758429579418342</v>
+        <v>3.501838080206315</v>
       </c>
       <c r="L21">
-        <v>1.694874496173247</v>
+        <v>3.496064890227895</v>
       </c>
       <c r="M21">
-        <v>1.121951512599277</v>
+        <v>5.249268226519737</v>
       </c>
       <c r="N21">
-        <v>1.121951512599277</v>
+        <v>5.249268226519737</v>
       </c>
       <c r="O21">
-        <v>1.469269830337761</v>
+        <v>3.500118080382877</v>
       </c>
       <c r="P21">
-        <v>0.7477148652063786</v>
+        <v>4.66679151108193</v>
       </c>
       <c r="Q21">
-        <v>0.7477148652063788</v>
+        <v>4.66679151108193</v>
       </c>
       <c r="R21">
-        <v>0.5605965415099294</v>
+        <v>4.375553153363026</v>
       </c>
       <c r="S21">
-        <v>0.5605965415099294</v>
+        <v>4.375553153363026</v>
       </c>
       <c r="T21">
-        <v>0.763962411240268</v>
+        <v>4.081096405100413</v>
       </c>
     </row>
     <row r="22" spans="1:20">
@@ -1822,58 +1828,58 @@
         <v>20</v>
       </c>
       <c r="C22">
-        <v>0.06949281876991974</v>
+        <v>0.001358614239473684</v>
       </c>
       <c r="D22">
-        <v>0.07529789264772963</v>
+        <v>6.778065580148422</v>
       </c>
       <c r="E22">
-        <v>0.4828810263023473</v>
+        <v>0.0009891908884210525</v>
       </c>
       <c r="F22">
-        <v>0.06949281876991974</v>
+        <v>0.001358614239473684</v>
       </c>
       <c r="G22">
-        <v>1.401767971530121</v>
+        <v>1.124473584028421</v>
       </c>
       <c r="H22">
-        <v>0.07529789264772963</v>
+        <v>6.778065580148422</v>
       </c>
       <c r="I22">
-        <v>-0.0004574272900550851</v>
+        <v>1.647539540644316</v>
       </c>
       <c r="J22">
-        <v>0.01587949993991768</v>
+        <v>0.01061339926157895</v>
       </c>
       <c r="K22">
-        <v>0.07529789264772963</v>
+        <v>6.778065580148422</v>
       </c>
       <c r="L22">
-        <v>0.4828810263023473</v>
+        <v>0.0009891908884210525</v>
       </c>
       <c r="M22">
-        <v>0.2761869225361335</v>
+        <v>0.001173902563947368</v>
       </c>
       <c r="N22">
-        <v>0.2761869225361335</v>
+        <v>0.001173902563947368</v>
       </c>
       <c r="O22">
-        <v>0.1839721392607373</v>
+        <v>0.5499624485907368</v>
       </c>
       <c r="P22">
-        <v>0.2092239125733323</v>
+        <v>2.260137795092105</v>
       </c>
       <c r="Q22">
-        <v>0.2092239125733323</v>
+        <v>2.260137795092105</v>
       </c>
       <c r="R22">
-        <v>0.1757424075919316</v>
+        <v>3.389619741356184</v>
       </c>
       <c r="S22">
-        <v>0.1757424075919316</v>
+        <v>3.389619741356184</v>
       </c>
       <c r="T22">
-        <v>0.3408102969833302</v>
+        <v>1.593839984868439</v>
       </c>
     </row>
     <row r="23" spans="1:20">
@@ -1884,58 +1890,58 @@
         <v>21</v>
       </c>
       <c r="C23">
-        <v>0.0009906382284935978</v>
+        <v>0.5490285290253076</v>
       </c>
       <c r="D23">
-        <v>1.650333686930785</v>
+        <v>-0.000758429579418342</v>
       </c>
       <c r="E23">
-        <v>0.9268749225926886</v>
+        <v>1.694874496173247</v>
       </c>
       <c r="F23">
-        <v>0.0009906382284935978</v>
+        <v>0.5490285290253076</v>
       </c>
       <c r="G23">
-        <v>2.22350904549545</v>
+        <v>0.09679846039972893</v>
       </c>
       <c r="H23">
-        <v>1.650333686930785</v>
+        <v>-0.000758429579418342</v>
       </c>
       <c r="I23">
-        <v>1.891613563536645</v>
+        <v>2.163906465814728</v>
       </c>
       <c r="J23">
-        <v>0.001147664018377604</v>
+        <v>0.07992494560801601</v>
       </c>
       <c r="K23">
-        <v>1.650333686930785</v>
+        <v>-0.000758429579418342</v>
       </c>
       <c r="L23">
-        <v>0.9268749225926886</v>
+        <v>1.694874496173247</v>
       </c>
       <c r="M23">
-        <v>0.4639327804105911</v>
+        <v>1.121951512599277</v>
       </c>
       <c r="N23">
-        <v>0.4639327804105911</v>
+        <v>1.121951512599277</v>
       </c>
       <c r="O23">
-        <v>0.9398263747859422</v>
+        <v>1.469269830337761</v>
       </c>
       <c r="P23">
-        <v>0.8593997492506559</v>
+        <v>0.7477148652063786</v>
       </c>
       <c r="Q23">
-        <v>0.8593997492506559</v>
+        <v>0.7477148652063788</v>
       </c>
       <c r="R23">
-        <v>1.057133233670688</v>
+        <v>0.5605965415099294</v>
       </c>
       <c r="S23">
-        <v>1.057133233670688</v>
+        <v>0.5605965415099294</v>
       </c>
       <c r="T23">
-        <v>1.11574492013374</v>
+        <v>0.763962411240268</v>
       </c>
     </row>
     <row r="24" spans="1:20">
@@ -1946,58 +1952,58 @@
         <v>22</v>
       </c>
       <c r="C24">
-        <v>3.806806310651667</v>
+        <v>0.06949281876991974</v>
       </c>
       <c r="D24">
-        <v>0.795381671876087</v>
+        <v>0.07529789264772963</v>
       </c>
       <c r="E24">
-        <v>1.257223936975514</v>
+        <v>0.4828810263023473</v>
       </c>
       <c r="F24">
-        <v>3.806806310651667</v>
+        <v>0.06949281876991974</v>
       </c>
       <c r="G24">
-        <v>1.380876313850261</v>
+        <v>1.401767971530121</v>
       </c>
       <c r="H24">
-        <v>0.795381671876087</v>
+        <v>0.07529789264772963</v>
       </c>
       <c r="I24">
-        <v>1.878161985072147</v>
+        <v>-0.0004574272900550851</v>
       </c>
       <c r="J24">
-        <v>2.492586044649239</v>
+        <v>0.01587949993991768</v>
       </c>
       <c r="K24">
-        <v>0.795381671876087</v>
+        <v>0.07529789264772963</v>
       </c>
       <c r="L24">
-        <v>1.257223936975514</v>
+        <v>0.4828810263023473</v>
       </c>
       <c r="M24">
-        <v>2.532015123813591</v>
+        <v>0.2761869225361335</v>
       </c>
       <c r="N24">
-        <v>2.532015123813591</v>
+        <v>0.2761869225361335</v>
       </c>
       <c r="O24">
-        <v>2.314064077566443</v>
+        <v>0.1839721392607373</v>
       </c>
       <c r="P24">
-        <v>1.95313730650109</v>
+        <v>0.2092239125733323</v>
       </c>
       <c r="Q24">
-        <v>1.953137306501089</v>
+        <v>0.2092239125733323</v>
       </c>
       <c r="R24">
-        <v>1.663698397844839</v>
+        <v>0.1757424075919316</v>
       </c>
       <c r="S24">
-        <v>1.663698397844839</v>
+        <v>0.1757424075919316</v>
       </c>
       <c r="T24">
-        <v>1.935172710512486</v>
+        <v>0.3408102969833302</v>
       </c>
     </row>
     <row r="25" spans="1:20">
@@ -2008,58 +2014,58 @@
         <v>23</v>
       </c>
       <c r="C25">
-        <v>0.0005785544083198467</v>
+        <v>0.0009906382284935978</v>
       </c>
       <c r="D25">
-        <v>0.9221787154030172</v>
+        <v>1.650333686930785</v>
       </c>
       <c r="E25">
-        <v>3.207764372415052</v>
+        <v>0.9268749225926886</v>
       </c>
       <c r="F25">
-        <v>0.0005785544083198467</v>
+        <v>0.0009906382284935978</v>
       </c>
       <c r="G25">
-        <v>0.01700950850845988</v>
+        <v>2.22350904549545</v>
       </c>
       <c r="H25">
-        <v>0.9221787154030172</v>
+        <v>1.650333686930785</v>
       </c>
       <c r="I25">
-        <v>0.006248484040885691</v>
+        <v>1.891613563536645</v>
       </c>
       <c r="J25">
-        <v>0.01141761173610538</v>
+        <v>0.001147664018377604</v>
       </c>
       <c r="K25">
-        <v>0.9221787154030172</v>
+        <v>1.650333686930785</v>
       </c>
       <c r="L25">
-        <v>3.207764372415052</v>
+        <v>0.9268749225926886</v>
       </c>
       <c r="M25">
-        <v>1.604171463411686</v>
+        <v>0.4639327804105911</v>
       </c>
       <c r="N25">
-        <v>1.604171463411686</v>
+        <v>0.4639327804105911</v>
       </c>
       <c r="O25">
-        <v>1.071530470288086</v>
+        <v>0.9398263747859422</v>
       </c>
       <c r="P25">
-        <v>1.376840547408796</v>
+        <v>0.8593997492506559</v>
       </c>
       <c r="Q25">
-        <v>1.376840547408796</v>
+        <v>0.8593997492506559</v>
       </c>
       <c r="R25">
-        <v>1.263175089407352</v>
+        <v>1.057133233670688</v>
       </c>
       <c r="S25">
-        <v>1.263175089407352</v>
+        <v>1.057133233670688</v>
       </c>
       <c r="T25">
-        <v>0.6941995410853067</v>
+        <v>1.11574492013374</v>
       </c>
     </row>
     <row r="26" spans="1:20">
@@ -2070,58 +2076,58 @@
         <v>24</v>
       </c>
       <c r="C26">
-        <v>0.003145952570695001</v>
+        <v>3.806806310651667</v>
       </c>
       <c r="D26">
-        <v>0.009635403838611055</v>
+        <v>0.795381671876087</v>
       </c>
       <c r="E26">
-        <v>1.276966659993725</v>
+        <v>1.257223936975514</v>
       </c>
       <c r="F26">
-        <v>0.003145952570695001</v>
+        <v>3.806806310651667</v>
       </c>
       <c r="G26">
-        <v>1.00617965130892</v>
+        <v>1.380876313850261</v>
       </c>
       <c r="H26">
-        <v>0.009635403838611055</v>
+        <v>0.795381671876087</v>
       </c>
       <c r="I26">
-        <v>0.5721374030175033</v>
+        <v>1.878161985072147</v>
       </c>
       <c r="J26">
-        <v>1.859767807519045</v>
+        <v>2.492586044649239</v>
       </c>
       <c r="K26">
-        <v>0.009635403838611055</v>
+        <v>0.795381671876087</v>
       </c>
       <c r="L26">
-        <v>1.276966659993725</v>
+        <v>1.257223936975514</v>
       </c>
       <c r="M26">
-        <v>0.64005630628221</v>
+        <v>2.532015123813591</v>
       </c>
       <c r="N26">
-        <v>0.64005630628221</v>
+        <v>2.532015123813591</v>
       </c>
       <c r="O26">
-        <v>0.6174166718606411</v>
+        <v>2.314064077566443</v>
       </c>
       <c r="P26">
-        <v>0.429916005467677</v>
+        <v>1.95313730650109</v>
       </c>
       <c r="Q26">
-        <v>0.429916005467677</v>
+        <v>1.953137306501089</v>
       </c>
       <c r="R26">
-        <v>0.3248458550604105</v>
+        <v>1.663698397844839</v>
       </c>
       <c r="S26">
-        <v>0.3248458550604105</v>
+        <v>1.663698397844839</v>
       </c>
       <c r="T26">
-        <v>0.7879721463747499</v>
+        <v>1.935172710512486</v>
       </c>
     </row>
     <row r="27" spans="1:20">
@@ -2132,58 +2138,58 @@
         <v>25</v>
       </c>
       <c r="C27">
-        <v>0.1226218843146754</v>
+        <v>0.0005785544083198467</v>
       </c>
       <c r="D27">
-        <v>1.145041287608157</v>
+        <v>0.9221787154030172</v>
       </c>
       <c r="E27">
-        <v>0.0008891324879004232</v>
+        <v>3.207764372415052</v>
       </c>
       <c r="F27">
-        <v>0.1226218843146754</v>
+        <v>0.0005785544083198467</v>
       </c>
       <c r="G27">
-        <v>0.4632761339827141</v>
+        <v>0.01700950850845988</v>
       </c>
       <c r="H27">
-        <v>1.145041287608157</v>
+        <v>0.9221787154030172</v>
       </c>
       <c r="I27">
-        <v>0.006069047697103314</v>
+        <v>0.006248484040885691</v>
       </c>
       <c r="J27">
-        <v>10.35736542542252</v>
+        <v>0.01141761173610538</v>
       </c>
       <c r="K27">
-        <v>1.145041287608157</v>
+        <v>0.9221787154030172</v>
       </c>
       <c r="L27">
-        <v>0.0008891324879004232</v>
+        <v>3.207764372415052</v>
       </c>
       <c r="M27">
-        <v>0.06175550840128793</v>
+        <v>1.604171463411686</v>
       </c>
       <c r="N27">
-        <v>0.06175550840128793</v>
+        <v>1.604171463411686</v>
       </c>
       <c r="O27">
-        <v>0.04319335483322639</v>
+        <v>1.071530470288086</v>
       </c>
       <c r="P27">
-        <v>0.4228507681369109</v>
+        <v>1.376840547408796</v>
       </c>
       <c r="Q27">
-        <v>0.4228507681369109</v>
+        <v>1.376840547408796</v>
       </c>
       <c r="R27">
-        <v>0.6033983980047224</v>
+        <v>1.263175089407352</v>
       </c>
       <c r="S27">
-        <v>0.6033983980047224</v>
+        <v>1.263175089407352</v>
       </c>
       <c r="T27">
-        <v>2.015877151918846</v>
+        <v>0.6941995410853067</v>
       </c>
     </row>
     <row r="28" spans="1:20">
@@ -2194,58 +2200,58 @@
         <v>26</v>
       </c>
       <c r="C28">
-        <v>0.03222520466330636</v>
+        <v>0.003145952570695001</v>
       </c>
       <c r="D28">
-        <v>0.029784882913573</v>
+        <v>0.009635403838611055</v>
       </c>
       <c r="E28">
-        <v>1.141624010106937</v>
+        <v>1.276966659993725</v>
       </c>
       <c r="F28">
-        <v>0.03222520466330636</v>
+        <v>0.003145952570695001</v>
       </c>
       <c r="G28">
-        <v>1.822320010950573</v>
+        <v>1.00617965130892</v>
       </c>
       <c r="H28">
-        <v>0.029784882913573</v>
+        <v>0.009635403838611055</v>
       </c>
       <c r="I28">
-        <v>1.404946126071093</v>
+        <v>0.5721374030175033</v>
       </c>
       <c r="J28">
-        <v>0.003689391777067894</v>
+        <v>1.859767807519045</v>
       </c>
       <c r="K28">
-        <v>0.029784882913573</v>
+        <v>0.009635403838611055</v>
       </c>
       <c r="L28">
-        <v>1.141624010106937</v>
+        <v>1.276966659993725</v>
       </c>
       <c r="M28">
-        <v>0.5869246073851218</v>
+        <v>0.64005630628221</v>
       </c>
       <c r="N28">
-        <v>0.5869246073851218</v>
+        <v>0.64005630628221</v>
       </c>
       <c r="O28">
-        <v>0.859598446947112</v>
+        <v>0.6174166718606411</v>
       </c>
       <c r="P28">
-        <v>0.4012113658946055</v>
+        <v>0.429916005467677</v>
       </c>
       <c r="Q28">
-        <v>0.4012113658946055</v>
+        <v>0.429916005467677</v>
       </c>
       <c r="R28">
-        <v>0.3083547451493474</v>
+        <v>0.3248458550604105</v>
       </c>
       <c r="S28">
-        <v>0.3083547451493474</v>
+        <v>0.3248458550604105</v>
       </c>
       <c r="T28">
-        <v>0.739098271080425</v>
+        <v>0.7879721463747499</v>
       </c>
     </row>
     <row r="29" spans="1:20">
@@ -2256,57 +2262,181 @@
         <v>27</v>
       </c>
       <c r="C29">
+        <v>0.1226218843146754</v>
+      </c>
+      <c r="D29">
+        <v>1.145041287608157</v>
+      </c>
+      <c r="E29">
+        <v>0.0008891324879004232</v>
+      </c>
+      <c r="F29">
+        <v>0.1226218843146754</v>
+      </c>
+      <c r="G29">
+        <v>0.4632761339827141</v>
+      </c>
+      <c r="H29">
+        <v>1.145041287608157</v>
+      </c>
+      <c r="I29">
+        <v>0.006069047697103314</v>
+      </c>
+      <c r="J29">
+        <v>10.35736542542252</v>
+      </c>
+      <c r="K29">
+        <v>1.145041287608157</v>
+      </c>
+      <c r="L29">
+        <v>0.0008891324879004232</v>
+      </c>
+      <c r="M29">
+        <v>0.06175550840128793</v>
+      </c>
+      <c r="N29">
+        <v>0.06175550840128793</v>
+      </c>
+      <c r="O29">
+        <v>0.04319335483322639</v>
+      </c>
+      <c r="P29">
+        <v>0.4228507681369109</v>
+      </c>
+      <c r="Q29">
+        <v>0.4228507681369109</v>
+      </c>
+      <c r="R29">
+        <v>0.6033983980047224</v>
+      </c>
+      <c r="S29">
+        <v>0.6033983980047224</v>
+      </c>
+      <c r="T29">
+        <v>2.015877151918846</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20">
+      <c r="A30" s="1">
+        <v>28</v>
+      </c>
+      <c r="B30" t="s">
+        <v>28</v>
+      </c>
+      <c r="C30">
+        <v>0.03222520466330636</v>
+      </c>
+      <c r="D30">
+        <v>0.029784882913573</v>
+      </c>
+      <c r="E30">
+        <v>1.141624010106937</v>
+      </c>
+      <c r="F30">
+        <v>0.03222520466330636</v>
+      </c>
+      <c r="G30">
+        <v>1.822320010950573</v>
+      </c>
+      <c r="H30">
+        <v>0.029784882913573</v>
+      </c>
+      <c r="I30">
+        <v>1.404946126071093</v>
+      </c>
+      <c r="J30">
+        <v>0.003689391777067894</v>
+      </c>
+      <c r="K30">
+        <v>0.029784882913573</v>
+      </c>
+      <c r="L30">
+        <v>1.141624010106937</v>
+      </c>
+      <c r="M30">
+        <v>0.5869246073851218</v>
+      </c>
+      <c r="N30">
+        <v>0.5869246073851218</v>
+      </c>
+      <c r="O30">
+        <v>0.859598446947112</v>
+      </c>
+      <c r="P30">
+        <v>0.4012113658946055</v>
+      </c>
+      <c r="Q30">
+        <v>0.4012113658946055</v>
+      </c>
+      <c r="R30">
+        <v>0.3083547451493474</v>
+      </c>
+      <c r="S30">
+        <v>0.3083547451493474</v>
+      </c>
+      <c r="T30">
+        <v>0.739098271080425</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20">
+      <c r="A31" s="1">
+        <v>29</v>
+      </c>
+      <c r="B31" t="s">
+        <v>29</v>
+      </c>
+      <c r="C31">
         <v>0.003650102051705286</v>
       </c>
-      <c r="D29">
+      <c r="D31">
         <v>-0.0007013616381167826</v>
       </c>
-      <c r="E29">
+      <c r="E31">
         <v>2.49730490468291</v>
       </c>
-      <c r="F29">
+      <c r="F31">
         <v>0.003650102051705286</v>
       </c>
-      <c r="G29">
+      <c r="G31">
         <v>0.7580881550873318</v>
       </c>
-      <c r="H29">
+      <c r="H31">
         <v>-0.0007013616381167826</v>
       </c>
-      <c r="I29">
+      <c r="I31">
         <v>2.893192146584329</v>
       </c>
-      <c r="J29">
+      <c r="J31">
         <v>-0.004807787644049314</v>
       </c>
-      <c r="K29">
+      <c r="K31">
         <v>-0.0007013616381167826</v>
       </c>
-      <c r="L29">
+      <c r="L31">
         <v>2.49730490468291</v>
       </c>
-      <c r="M29">
+      <c r="M31">
         <v>1.250477503367307</v>
       </c>
-      <c r="N29">
+      <c r="N31">
         <v>1.250477503367307</v>
       </c>
-      <c r="O29">
+      <c r="O31">
         <v>1.798049051106315</v>
       </c>
-      <c r="P29">
+      <c r="P31">
         <v>0.8334178816988328</v>
       </c>
-      <c r="Q29">
+      <c r="Q31">
         <v>0.8334178816988328</v>
       </c>
-      <c r="R29">
+      <c r="R31">
         <v>0.6248880708645954</v>
       </c>
-      <c r="S29">
+      <c r="S31">
         <v>0.6248880708645954</v>
       </c>
-      <c r="T29">
+      <c r="T31">
         <v>1.024454359854018</v>
       </c>
     </row>

</xml_diff>